<commit_message>
added date_created timestamp default now()
</commit_message>
<xml_diff>
--- a/tmp/LA DCs Order Guide.xlsx
+++ b/tmp/LA DCs Order Guide.xlsx
@@ -14,7 +14,9 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'BB 10 15 2018'!$A$1:$L$114</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles" vbProcedure="false">'BB 10 15 2018'!$1:$8</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'BB 10 15 2018'!$A$1:$L$114</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'BB 10 15 2018'!$A$1:$L$114</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles" vbProcedure="false">'BB 10 15 2018'!$1:$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0" vbProcedure="false">'BB 10 15 2018'!$1:$8</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -591,12 +593,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -725,6 +721,12 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="11"/>
       <name val="Microsoft YaHei"/>
       <family val="2"/>
@@ -864,12 +866,12 @@
     </xf>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="63">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -878,27 +880,27 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -910,103 +912,99 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="3" borderId="3" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="3" borderId="2" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="15" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="3" borderId="3" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="6" fillId="3" borderId="2" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="16" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1018,88 +1016,84 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="4" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="4" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="22" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1110,59 +1104,19 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="170" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="170" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -1178,7 +1132,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Normal 2" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1251,15 +1205,15 @@
   <dimension ref="A1:L114"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L6" activeCellId="0" sqref="L6"/>
+      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.31983805668016"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.6761133603239"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="70.9109311740891"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.7813765182186"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="71.4493927125506"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.4251012145749"/>
     <col collapsed="false" hidden="false" max="12" min="6" style="1" width="13.6032388663968"/>
     <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.57085020242915"/>
@@ -1329,2514 +1283,2514 @@
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="9"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="14" t="s">
+      <c r="D5" s="11"/>
+      <c r="E5" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="9"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="15" t="s">
+      <c r="D6" s="11"/>
+      <c r="E6" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="16" t="n">
-        <v>43398</v>
-      </c>
-      <c r="G6" s="17" t="n">
+      <c r="F6" s="15" t="n">
+        <v>43404</v>
+      </c>
+      <c r="G6" s="16" t="n">
         <f aca="false">F6+1</f>
-        <v>43399</v>
-      </c>
-      <c r="H6" s="16" t="n">
+        <v>43405</v>
+      </c>
+      <c r="H6" s="15" t="n">
         <f aca="false">+G6+1</f>
-        <v>43400</v>
-      </c>
-      <c r="I6" s="17" t="n">
+        <v>43406</v>
+      </c>
+      <c r="I6" s="16" t="n">
         <f aca="false">+H6+1</f>
-        <v>43401</v>
-      </c>
-      <c r="J6" s="16" t="n">
+        <v>43407</v>
+      </c>
+      <c r="J6" s="15" t="n">
         <f aca="false">+I6+1</f>
-        <v>43402</v>
-      </c>
-      <c r="K6" s="17" t="n">
+        <v>43408</v>
+      </c>
+      <c r="K6" s="16" t="n">
         <f aca="false">+J6+1</f>
-        <v>43403</v>
-      </c>
-      <c r="L6" s="16" t="n">
+        <v>43409</v>
+      </c>
+      <c r="L6" s="15" t="n">
         <f aca="false">+K6+1</f>
-        <v>43404</v>
+        <v>43410</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="9"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="15" t="s">
+      <c r="D7" s="11"/>
+      <c r="E7" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="16" t="n">
+      <c r="F7" s="15" t="n">
         <f aca="false">F6+2</f>
-        <v>43400</v>
-      </c>
-      <c r="G7" s="17" t="n">
+        <v>43406</v>
+      </c>
+      <c r="G7" s="16" t="n">
         <f aca="false">G6+2</f>
-        <v>43401</v>
-      </c>
-      <c r="H7" s="16" t="n">
+        <v>43407</v>
+      </c>
+      <c r="H7" s="15" t="n">
         <f aca="false">H6+2</f>
-        <v>43402</v>
-      </c>
-      <c r="I7" s="17" t="n">
+        <v>43408</v>
+      </c>
+      <c r="I7" s="16" t="n">
         <f aca="false">I6+2</f>
-        <v>43403</v>
-      </c>
-      <c r="J7" s="16" t="n">
+        <v>43409</v>
+      </c>
+      <c r="J7" s="15" t="n">
         <f aca="false">J6+2</f>
-        <v>43404</v>
-      </c>
-      <c r="K7" s="17" t="n">
+        <v>43410</v>
+      </c>
+      <c r="K7" s="16" t="n">
         <f aca="false">K6+2</f>
-        <v>43405</v>
-      </c>
-      <c r="L7" s="16" t="n">
+        <v>43411</v>
+      </c>
+      <c r="L7" s="15" t="n">
         <f aca="false">L6+2</f>
-        <v>43406</v>
+        <v>43412</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="21"/>
-      <c r="F8" s="22" t="s">
+      <c r="E8" s="20"/>
+      <c r="F8" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="22" t="s">
+      <c r="G8" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="22" t="s">
+      <c r="H8" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="I8" s="22" t="s">
+      <c r="I8" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="J8" s="22" t="s">
+      <c r="J8" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="K8" s="22" t="s">
+      <c r="K8" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="L8" s="22" t="s">
+      <c r="L8" s="21" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="23"/>
-      <c r="B9" s="24"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="26" t="s">
+      <c r="A9" s="22"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="27"/>
-      <c r="F9" s="28" t="n">
+      <c r="E9" s="26"/>
+      <c r="F9" s="27" t="n">
         <f aca="false">SUM(F10:F114)</f>
         <v>9</v>
       </c>
-      <c r="G9" s="28" t="n">
+      <c r="G9" s="27" t="n">
         <f aca="false">SUM(G10:G114)</f>
         <v>11</v>
       </c>
-      <c r="H9" s="28" t="n">
+      <c r="H9" s="27" t="n">
         <f aca="false">SUM(H10:H114)</f>
         <v>13</v>
       </c>
-      <c r="I9" s="28" t="n">
+      <c r="I9" s="27" t="n">
         <f aca="false">SUM(I10:I114)</f>
         <v>15</v>
       </c>
-      <c r="J9" s="28" t="n">
+      <c r="J9" s="27" t="n">
         <f aca="false">SUM(J10:J114)</f>
         <v>17</v>
       </c>
-      <c r="K9" s="28" t="n">
+      <c r="K9" s="27" t="n">
         <f aca="false">SUM(K10:K114)</f>
         <v>19</v>
       </c>
-      <c r="L9" s="28" t="n">
+      <c r="L9" s="27" t="n">
         <f aca="false">SUM(L10:L114)</f>
         <v>21</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="9"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="30" t="s">
+      <c r="C10" s="28"/>
+      <c r="D10" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="31"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="33"/>
-      <c r="H10" s="33"/>
-      <c r="I10" s="33"/>
-      <c r="J10" s="32"/>
-      <c r="K10" s="33"/>
-      <c r="L10" s="34"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="32"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="32"/>
+      <c r="L10" s="33"/>
     </row>
     <row r="11" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="35" t="n">
+      <c r="A11" s="34" t="n">
         <v>1.38</v>
       </c>
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="37" t="n">
+      <c r="C11" s="36" t="n">
         <v>50728</v>
       </c>
-      <c r="D11" s="38" t="s">
+      <c r="D11" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="38" t="s">
+      <c r="E11" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="F11" s="39" t="n">
+      <c r="F11" s="38" t="n">
         <v>1</v>
       </c>
-      <c r="G11" s="39"/>
-      <c r="H11" s="39"/>
-      <c r="I11" s="39"/>
-      <c r="J11" s="39"/>
-      <c r="K11" s="39"/>
-      <c r="L11" s="39"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="38"/>
+      <c r="J11" s="38"/>
+      <c r="K11" s="38"/>
+      <c r="L11" s="38"/>
     </row>
     <row r="12" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="35" t="n">
+      <c r="A12" s="34" t="n">
         <v>1.38</v>
       </c>
-      <c r="B12" s="36" t="s">
+      <c r="B12" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="37" t="n">
+      <c r="C12" s="36" t="n">
         <v>50729</v>
       </c>
-      <c r="D12" s="40" t="s">
+      <c r="D12" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="E12" s="40" t="s">
+      <c r="E12" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="F12" s="39"/>
-      <c r="G12" s="39" t="n">
+      <c r="F12" s="38"/>
+      <c r="G12" s="38" t="n">
         <v>2</v>
       </c>
-      <c r="H12" s="39"/>
-      <c r="I12" s="39"/>
-      <c r="J12" s="39"/>
-      <c r="K12" s="39"/>
-      <c r="L12" s="39"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="38"/>
+      <c r="L12" s="38"/>
     </row>
     <row r="13" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="35" t="n">
+      <c r="A13" s="34" t="n">
         <v>1.38</v>
       </c>
-      <c r="B13" s="36" t="s">
+      <c r="B13" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="37" t="n">
+      <c r="C13" s="36" t="n">
         <v>50730</v>
       </c>
-      <c r="D13" s="40" t="s">
+      <c r="D13" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="40" t="s">
+      <c r="E13" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="41"/>
-      <c r="G13" s="42"/>
-      <c r="H13" s="42" t="n">
+      <c r="F13" s="40"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="41" t="n">
         <v>3</v>
       </c>
-      <c r="I13" s="42"/>
-      <c r="J13" s="41"/>
-      <c r="K13" s="42"/>
-      <c r="L13" s="41"/>
+      <c r="I13" s="41"/>
+      <c r="J13" s="40"/>
+      <c r="K13" s="41"/>
+      <c r="L13" s="40"/>
     </row>
     <row r="14" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="35" t="n">
+      <c r="A14" s="34" t="n">
         <v>1.38</v>
       </c>
-      <c r="B14" s="36" t="s">
+      <c r="B14" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="37" t="n">
+      <c r="C14" s="36" t="n">
         <v>50731</v>
       </c>
-      <c r="D14" s="43" t="s">
+      <c r="D14" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="E14" s="43" t="s">
+      <c r="E14" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="F14" s="39"/>
-      <c r="G14" s="39"/>
-      <c r="H14" s="39"/>
-      <c r="I14" s="39" t="n">
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38" t="n">
         <v>4</v>
       </c>
-      <c r="J14" s="39"/>
-      <c r="K14" s="39"/>
-      <c r="L14" s="39"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="38"/>
+      <c r="L14" s="38"/>
     </row>
     <row r="15" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="35" t="n">
+      <c r="A15" s="34" t="n">
         <v>1.38</v>
       </c>
-      <c r="B15" s="36" t="s">
+      <c r="B15" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="44" t="n">
+      <c r="C15" s="43" t="n">
         <v>50732</v>
       </c>
-      <c r="D15" s="45" t="s">
+      <c r="D15" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="E15" s="46" t="s">
+      <c r="E15" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="F15" s="39"/>
-      <c r="G15" s="39"/>
-      <c r="H15" s="39"/>
-      <c r="I15" s="39"/>
-      <c r="J15" s="39" t="n">
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="38"/>
+      <c r="J15" s="38" t="n">
         <v>5</v>
       </c>
-      <c r="K15" s="39"/>
-      <c r="L15" s="39"/>
+      <c r="K15" s="38"/>
+      <c r="L15" s="38"/>
     </row>
     <row r="16" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="35" t="n">
+      <c r="A16" s="34" t="n">
         <v>1.38</v>
       </c>
-      <c r="B16" s="36" t="s">
+      <c r="B16" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="37" t="n">
+      <c r="C16" s="36" t="n">
         <v>50733</v>
       </c>
-      <c r="D16" s="43" t="s">
+      <c r="D16" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="E16" s="43" t="s">
+      <c r="E16" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="F16" s="39"/>
-      <c r="G16" s="39"/>
-      <c r="H16" s="39"/>
-      <c r="I16" s="39"/>
-      <c r="J16" s="39"/>
-      <c r="K16" s="39" t="n">
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38"/>
+      <c r="J16" s="38"/>
+      <c r="K16" s="38" t="n">
         <v>6</v>
       </c>
-      <c r="L16" s="39"/>
+      <c r="L16" s="38"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="35"/>
-      <c r="B17" s="36"/>
-      <c r="C17" s="29"/>
-      <c r="D17" s="30" t="s">
+      <c r="A17" s="34"/>
+      <c r="B17" s="35"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="E17" s="31"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="33"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="33"/>
-      <c r="J17" s="32"/>
-      <c r="K17" s="33"/>
-      <c r="L17" s="34"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="32"/>
+      <c r="J17" s="31"/>
+      <c r="K17" s="32"/>
+      <c r="L17" s="33"/>
     </row>
     <row r="18" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="35" t="n">
+      <c r="A18" s="34" t="n">
         <v>1.84</v>
       </c>
-      <c r="B18" s="36" t="s">
+      <c r="B18" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="37" t="n">
+      <c r="C18" s="36" t="n">
         <v>50734</v>
       </c>
-      <c r="D18" s="40" t="s">
+      <c r="D18" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="E18" s="40" t="s">
+      <c r="E18" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="F18" s="39"/>
-      <c r="G18" s="39"/>
-      <c r="H18" s="39"/>
-      <c r="I18" s="39"/>
-      <c r="J18" s="39"/>
-      <c r="K18" s="39"/>
-      <c r="L18" s="39" t="n">
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="38"/>
+      <c r="J18" s="38"/>
+      <c r="K18" s="38"/>
+      <c r="L18" s="38" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="35" t="n">
+      <c r="A19" s="34" t="n">
         <v>1.84</v>
       </c>
-      <c r="B19" s="36" t="s">
+      <c r="B19" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="44" t="n">
+      <c r="C19" s="43" t="n">
         <v>11060</v>
       </c>
-      <c r="D19" s="47" t="s">
+      <c r="D19" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="E19" s="40" t="s">
+      <c r="E19" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="F19" s="39" t="n">
+      <c r="F19" s="38" t="n">
         <v>8</v>
       </c>
-      <c r="G19" s="39"/>
-      <c r="H19" s="39"/>
-      <c r="I19" s="39"/>
-      <c r="J19" s="39"/>
-      <c r="K19" s="39"/>
-      <c r="L19" s="39"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="38"/>
+      <c r="I19" s="38"/>
+      <c r="J19" s="38"/>
+      <c r="K19" s="38"/>
+      <c r="L19" s="38"/>
     </row>
     <row r="20" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="35" t="n">
+      <c r="A20" s="34" t="n">
         <v>1.84</v>
       </c>
-      <c r="B20" s="36" t="s">
+      <c r="B20" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="44" t="n">
+      <c r="C20" s="43" t="n">
         <v>11061</v>
       </c>
-      <c r="D20" s="47" t="s">
+      <c r="D20" s="46" t="s">
         <v>40</v>
       </c>
-      <c r="E20" s="40" t="s">
+      <c r="E20" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="F20" s="39"/>
-      <c r="G20" s="39" t="n">
+      <c r="F20" s="38"/>
+      <c r="G20" s="38" t="n">
         <v>9</v>
       </c>
-      <c r="H20" s="39"/>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
-      <c r="K20" s="39"/>
-      <c r="L20" s="39"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="38"/>
+      <c r="J20" s="38"/>
+      <c r="K20" s="38"/>
+      <c r="L20" s="38"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="35"/>
-      <c r="B21" s="36"/>
-      <c r="C21" s="48"/>
-      <c r="D21" s="49" t="s">
+      <c r="A21" s="34"/>
+      <c r="B21" s="35"/>
+      <c r="C21" s="47"/>
+      <c r="D21" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="E21" s="50"/>
-      <c r="F21" s="41"/>
-      <c r="G21" s="42"/>
-      <c r="H21" s="42"/>
-      <c r="I21" s="42"/>
-      <c r="J21" s="41"/>
-      <c r="K21" s="42"/>
-      <c r="L21" s="41"/>
+      <c r="E21" s="49"/>
+      <c r="F21" s="40"/>
+      <c r="G21" s="41"/>
+      <c r="H21" s="41"/>
+      <c r="I21" s="41"/>
+      <c r="J21" s="40"/>
+      <c r="K21" s="41"/>
+      <c r="L21" s="40"/>
     </row>
     <row r="22" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="35" t="n">
+      <c r="A22" s="34" t="n">
         <v>1.38</v>
       </c>
-      <c r="B22" s="36" t="s">
+      <c r="B22" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C22" s="44" t="n">
+      <c r="C22" s="43" t="n">
         <v>11072</v>
       </c>
-      <c r="D22" s="43" t="s">
+      <c r="D22" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="E22" s="40" t="s">
+      <c r="E22" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="F22" s="39"/>
-      <c r="G22" s="39"/>
-      <c r="H22" s="39" t="n">
+      <c r="F22" s="38"/>
+      <c r="G22" s="38"/>
+      <c r="H22" s="38" t="n">
         <v>10</v>
       </c>
-      <c r="I22" s="39"/>
-      <c r="J22" s="39"/>
-      <c r="K22" s="39"/>
-      <c r="L22" s="39"/>
+      <c r="I22" s="38"/>
+      <c r="J22" s="38"/>
+      <c r="K22" s="38"/>
+      <c r="L22" s="38"/>
     </row>
     <row r="23" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="35" t="n">
+      <c r="A23" s="34" t="n">
         <v>1.38</v>
       </c>
-      <c r="B23" s="36" t="s">
+      <c r="B23" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C23" s="44" t="n">
+      <c r="C23" s="43" t="n">
         <v>11075</v>
       </c>
-      <c r="D23" s="43" t="s">
+      <c r="D23" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="E23" s="40" t="s">
+      <c r="E23" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="F23" s="39"/>
-      <c r="G23" s="39"/>
-      <c r="H23" s="39"/>
-      <c r="I23" s="39" t="n">
+      <c r="F23" s="38"/>
+      <c r="G23" s="38"/>
+      <c r="H23" s="38"/>
+      <c r="I23" s="38" t="n">
         <v>11</v>
       </c>
-      <c r="J23" s="39"/>
-      <c r="K23" s="39"/>
-      <c r="L23" s="39"/>
+      <c r="J23" s="38"/>
+      <c r="K23" s="38"/>
+      <c r="L23" s="38"/>
     </row>
     <row r="24" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="35" t="n">
+      <c r="A24" s="34" t="n">
         <v>1.84</v>
       </c>
-      <c r="B24" s="36" t="s">
+      <c r="B24" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C24" s="44" t="n">
+      <c r="C24" s="43" t="n">
         <v>11130</v>
       </c>
-      <c r="D24" s="43" t="s">
+      <c r="D24" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="E24" s="40" t="s">
+      <c r="E24" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="F24" s="39"/>
-      <c r="G24" s="39"/>
-      <c r="H24" s="39"/>
-      <c r="I24" s="39"/>
-      <c r="J24" s="39" t="n">
+      <c r="F24" s="38"/>
+      <c r="G24" s="38"/>
+      <c r="H24" s="38"/>
+      <c r="I24" s="38"/>
+      <c r="J24" s="38" t="n">
         <v>12</v>
       </c>
-      <c r="K24" s="39"/>
-      <c r="L24" s="39"/>
+      <c r="K24" s="38"/>
+      <c r="L24" s="38"/>
     </row>
     <row r="25" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="35" t="n">
+      <c r="A25" s="34" t="n">
         <v>1.84</v>
       </c>
-      <c r="B25" s="36" t="s">
+      <c r="B25" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="44" t="n">
+      <c r="C25" s="43" t="n">
         <v>11074</v>
       </c>
-      <c r="D25" s="43" t="s">
+      <c r="D25" s="42" t="s">
         <v>45</v>
       </c>
-      <c r="E25" s="40" t="s">
+      <c r="E25" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="F25" s="39"/>
-      <c r="G25" s="39"/>
-      <c r="H25" s="39"/>
-      <c r="I25" s="39"/>
-      <c r="J25" s="39"/>
-      <c r="K25" s="39" t="n">
+      <c r="F25" s="38"/>
+      <c r="G25" s="38"/>
+      <c r="H25" s="38"/>
+      <c r="I25" s="38"/>
+      <c r="J25" s="38"/>
+      <c r="K25" s="38" t="n">
         <v>13</v>
       </c>
-      <c r="L25" s="39"/>
+      <c r="L25" s="38"/>
     </row>
     <row r="26" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="35" t="n">
+      <c r="A26" s="34" t="n">
         <v>1.84</v>
       </c>
-      <c r="B26" s="36" t="s">
+      <c r="B26" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C26" s="44" t="n">
+      <c r="C26" s="43" t="n">
         <v>11071</v>
       </c>
-      <c r="D26" s="47" t="s">
+      <c r="D26" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="E26" s="40" t="s">
+      <c r="E26" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="F26" s="39"/>
-      <c r="G26" s="39"/>
-      <c r="H26" s="39"/>
-      <c r="I26" s="39"/>
-      <c r="J26" s="39"/>
-      <c r="K26" s="39"/>
-      <c r="L26" s="39" t="n">
+      <c r="F26" s="38"/>
+      <c r="G26" s="38"/>
+      <c r="H26" s="38"/>
+      <c r="I26" s="38"/>
+      <c r="J26" s="38"/>
+      <c r="K26" s="38"/>
+      <c r="L26" s="38" t="n">
         <v>14</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="35"/>
-      <c r="B27" s="36"/>
-      <c r="C27" s="48"/>
-      <c r="D27" s="49" t="s">
+      <c r="A27" s="34"/>
+      <c r="B27" s="35"/>
+      <c r="C27" s="47"/>
+      <c r="D27" s="48" t="s">
         <v>47</v>
       </c>
-      <c r="E27" s="50"/>
-      <c r="F27" s="41"/>
-      <c r="G27" s="42"/>
-      <c r="H27" s="42"/>
-      <c r="I27" s="42"/>
-      <c r="J27" s="41"/>
-      <c r="K27" s="42"/>
-      <c r="L27" s="41"/>
+      <c r="E27" s="49"/>
+      <c r="F27" s="40"/>
+      <c r="G27" s="41"/>
+      <c r="H27" s="41"/>
+      <c r="I27" s="41"/>
+      <c r="J27" s="40"/>
+      <c r="K27" s="41"/>
+      <c r="L27" s="40"/>
     </row>
     <row r="28" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="35" t="n">
+      <c r="A28" s="34" t="n">
         <v>1.84</v>
       </c>
-      <c r="B28" s="36" t="s">
+      <c r="B28" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="C28" s="37" t="n">
+      <c r="C28" s="36" t="n">
         <v>50742</v>
       </c>
-      <c r="D28" s="51" t="s">
+      <c r="D28" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="E28" s="40" t="s">
+      <c r="E28" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="F28" s="39"/>
-      <c r="G28" s="39"/>
-      <c r="H28" s="39"/>
-      <c r="I28" s="39"/>
-      <c r="J28" s="39"/>
-      <c r="K28" s="39"/>
-      <c r="L28" s="39"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="38"/>
+      <c r="K28" s="38"/>
+      <c r="L28" s="38"/>
     </row>
     <row r="29" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="35" t="n">
+      <c r="A29" s="34" t="n">
         <v>1.84</v>
       </c>
-      <c r="B29" s="36" t="s">
+      <c r="B29" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="C29" s="37" t="n">
+      <c r="C29" s="36" t="n">
         <v>50743</v>
       </c>
-      <c r="D29" s="51" t="s">
+      <c r="D29" s="50" t="s">
         <v>50</v>
       </c>
-      <c r="E29" s="40" t="s">
+      <c r="E29" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
-      <c r="K29" s="39"/>
-      <c r="L29" s="39"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="38"/>
+      <c r="I29" s="38"/>
+      <c r="J29" s="38"/>
+      <c r="K29" s="38"/>
+      <c r="L29" s="38"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="35"/>
-      <c r="B30" s="36"/>
-      <c r="C30" s="48"/>
-      <c r="D30" s="49" t="s">
+      <c r="A30" s="34"/>
+      <c r="B30" s="35"/>
+      <c r="C30" s="47"/>
+      <c r="D30" s="48" t="s">
         <v>51</v>
       </c>
-      <c r="E30" s="50"/>
-      <c r="F30" s="41"/>
-      <c r="G30" s="42"/>
-      <c r="H30" s="42"/>
-      <c r="I30" s="42"/>
-      <c r="J30" s="41"/>
-      <c r="K30" s="42"/>
-      <c r="L30" s="41"/>
+      <c r="E30" s="49"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="41"/>
+      <c r="H30" s="41"/>
+      <c r="I30" s="41"/>
+      <c r="J30" s="40"/>
+      <c r="K30" s="41"/>
+      <c r="L30" s="40"/>
     </row>
     <row r="31" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="35" t="n">
+      <c r="A31" s="34" t="n">
         <v>1.38</v>
       </c>
-      <c r="B31" s="36" t="s">
+      <c r="B31" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="C31" s="37" t="n">
+      <c r="C31" s="36" t="n">
         <v>50744</v>
       </c>
-      <c r="D31" s="40" t="s">
+      <c r="D31" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="E31" s="40" t="s">
+      <c r="E31" s="39" t="s">
         <v>53</v>
       </c>
-      <c r="F31" s="39"/>
-      <c r="G31" s="39"/>
-      <c r="H31" s="39"/>
-      <c r="I31" s="39"/>
-      <c r="J31" s="39"/>
-      <c r="K31" s="39"/>
-      <c r="L31" s="39"/>
+      <c r="F31" s="38"/>
+      <c r="G31" s="38"/>
+      <c r="H31" s="38"/>
+      <c r="I31" s="38"/>
+      <c r="J31" s="38"/>
+      <c r="K31" s="38"/>
+      <c r="L31" s="38"/>
     </row>
     <row r="32" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="35" t="n">
+      <c r="A32" s="34" t="n">
         <v>1.38</v>
       </c>
-      <c r="B32" s="36" t="s">
+      <c r="B32" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="C32" s="37" t="n">
+      <c r="C32" s="36" t="n">
         <v>50745</v>
       </c>
-      <c r="D32" s="40" t="s">
+      <c r="D32" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="E32" s="40" t="s">
+      <c r="E32" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="F32" s="39"/>
-      <c r="G32" s="39"/>
-      <c r="H32" s="39"/>
-      <c r="I32" s="39"/>
-      <c r="J32" s="39"/>
-      <c r="K32" s="39"/>
-      <c r="L32" s="39"/>
+      <c r="F32" s="38"/>
+      <c r="G32" s="38"/>
+      <c r="H32" s="38"/>
+      <c r="I32" s="38"/>
+      <c r="J32" s="38"/>
+      <c r="K32" s="38"/>
+      <c r="L32" s="38"/>
     </row>
     <row r="33" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="35" t="n">
+      <c r="A33" s="34" t="n">
         <v>1.38</v>
       </c>
-      <c r="B33" s="36" t="s">
+      <c r="B33" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="C33" s="37" t="n">
+      <c r="C33" s="36" t="n">
         <v>50746</v>
       </c>
-      <c r="D33" s="51" t="s">
+      <c r="D33" s="50" t="s">
         <v>56</v>
       </c>
-      <c r="E33" s="40" t="s">
+      <c r="E33" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="F33" s="39"/>
-      <c r="G33" s="39"/>
-      <c r="H33" s="39"/>
-      <c r="I33" s="39"/>
-      <c r="J33" s="39"/>
-      <c r="K33" s="39"/>
-      <c r="L33" s="39"/>
+      <c r="F33" s="38"/>
+      <c r="G33" s="38"/>
+      <c r="H33" s="38"/>
+      <c r="I33" s="38"/>
+      <c r="J33" s="38"/>
+      <c r="K33" s="38"/>
+      <c r="L33" s="38"/>
     </row>
     <row r="34" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="35" t="n">
+      <c r="A34" s="34" t="n">
         <v>1.38</v>
       </c>
-      <c r="B34" s="36" t="s">
+      <c r="B34" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="C34" s="37" t="n">
+      <c r="C34" s="36" t="n">
         <v>50747</v>
       </c>
-      <c r="D34" s="40" t="s">
+      <c r="D34" s="39" t="s">
         <v>58</v>
       </c>
-      <c r="E34" s="40" t="s">
+      <c r="E34" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="F34" s="39"/>
-      <c r="G34" s="39"/>
-      <c r="H34" s="39"/>
-      <c r="I34" s="39"/>
-      <c r="J34" s="39"/>
-      <c r="K34" s="39"/>
-      <c r="L34" s="39"/>
+      <c r="F34" s="38"/>
+      <c r="G34" s="38"/>
+      <c r="H34" s="38"/>
+      <c r="I34" s="38"/>
+      <c r="J34" s="38"/>
+      <c r="K34" s="38"/>
+      <c r="L34" s="38"/>
     </row>
     <row r="35" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="35" t="n">
+      <c r="A35" s="34" t="n">
         <v>1.38</v>
       </c>
-      <c r="B35" s="36" t="s">
+      <c r="B35" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="C35" s="37" t="n">
+      <c r="C35" s="36" t="n">
         <v>50748</v>
       </c>
-      <c r="D35" s="51" t="s">
+      <c r="D35" s="50" t="s">
         <v>60</v>
       </c>
-      <c r="E35" s="40" t="s">
+      <c r="E35" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="F35" s="39"/>
-      <c r="G35" s="39"/>
-      <c r="H35" s="39"/>
-      <c r="I35" s="39"/>
-      <c r="J35" s="39"/>
-      <c r="K35" s="39"/>
-      <c r="L35" s="39"/>
+      <c r="F35" s="38"/>
+      <c r="G35" s="38"/>
+      <c r="H35" s="38"/>
+      <c r="I35" s="38"/>
+      <c r="J35" s="38"/>
+      <c r="K35" s="38"/>
+      <c r="L35" s="38"/>
     </row>
     <row r="36" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="35" t="n">
+      <c r="A36" s="34" t="n">
         <v>1.38</v>
       </c>
-      <c r="B36" s="36" t="s">
+      <c r="B36" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="C36" s="37" t="n">
+      <c r="C36" s="36" t="n">
         <v>50749</v>
       </c>
-      <c r="D36" s="40" t="s">
+      <c r="D36" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="E36" s="40" t="s">
+      <c r="E36" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="F36" s="39"/>
-      <c r="G36" s="39"/>
-      <c r="H36" s="39"/>
-      <c r="I36" s="39"/>
-      <c r="J36" s="39"/>
-      <c r="K36" s="39"/>
-      <c r="L36" s="39"/>
+      <c r="F36" s="38"/>
+      <c r="G36" s="38"/>
+      <c r="H36" s="38"/>
+      <c r="I36" s="38"/>
+      <c r="J36" s="38"/>
+      <c r="K36" s="38"/>
+      <c r="L36" s="38"/>
     </row>
     <row r="37" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="35" t="n">
+      <c r="A37" s="34" t="n">
         <v>1.38</v>
       </c>
-      <c r="B37" s="36" t="s">
+      <c r="B37" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="C37" s="37" t="n">
+      <c r="C37" s="36" t="n">
         <v>50750</v>
       </c>
-      <c r="D37" s="40" t="s">
+      <c r="D37" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="E37" s="40" t="s">
+      <c r="E37" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="F37" s="39"/>
-      <c r="G37" s="39"/>
-      <c r="H37" s="39"/>
-      <c r="I37" s="39"/>
-      <c r="J37" s="39"/>
-      <c r="K37" s="39"/>
-      <c r="L37" s="39"/>
+      <c r="F37" s="38"/>
+      <c r="G37" s="38"/>
+      <c r="H37" s="38"/>
+      <c r="I37" s="38"/>
+      <c r="J37" s="38"/>
+      <c r="K37" s="38"/>
+      <c r="L37" s="38"/>
     </row>
     <row r="38" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="35" t="n">
+      <c r="A38" s="34" t="n">
         <v>1.38</v>
       </c>
-      <c r="B38" s="36" t="s">
+      <c r="B38" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="C38" s="37" t="n">
+      <c r="C38" s="36" t="n">
         <v>50751</v>
       </c>
-      <c r="D38" s="52" t="s">
+      <c r="D38" s="51" t="s">
         <v>63</v>
       </c>
-      <c r="E38" s="40" t="s">
+      <c r="E38" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="F38" s="39"/>
-      <c r="G38" s="39"/>
-      <c r="H38" s="39"/>
-      <c r="I38" s="39"/>
-      <c r="J38" s="39"/>
-      <c r="K38" s="39"/>
-      <c r="L38" s="39"/>
+      <c r="F38" s="38"/>
+      <c r="G38" s="38"/>
+      <c r="H38" s="38"/>
+      <c r="I38" s="38"/>
+      <c r="J38" s="38"/>
+      <c r="K38" s="38"/>
+      <c r="L38" s="38"/>
     </row>
     <row r="39" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="35" t="n">
+      <c r="A39" s="34" t="n">
         <v>1.84</v>
       </c>
-      <c r="B39" s="36" t="s">
+      <c r="B39" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C39" s="37" t="n">
+      <c r="C39" s="36" t="n">
         <v>50752</v>
       </c>
-      <c r="D39" s="52" t="s">
+      <c r="D39" s="51" t="s">
         <v>65</v>
       </c>
-      <c r="E39" s="40" t="s">
+      <c r="E39" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="F39" s="41"/>
-      <c r="G39" s="42"/>
-      <c r="H39" s="42"/>
-      <c r="I39" s="42"/>
-      <c r="J39" s="41"/>
-      <c r="K39" s="42"/>
-      <c r="L39" s="41"/>
+      <c r="F39" s="40"/>
+      <c r="G39" s="41"/>
+      <c r="H39" s="41"/>
+      <c r="I39" s="41"/>
+      <c r="J39" s="40"/>
+      <c r="K39" s="41"/>
+      <c r="L39" s="40"/>
     </row>
     <row r="40" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="35" t="n">
+      <c r="A40" s="34" t="n">
         <v>1.84</v>
       </c>
-      <c r="B40" s="36" t="s">
+      <c r="B40" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C40" s="37" t="n">
+      <c r="C40" s="36" t="n">
         <v>50753</v>
       </c>
-      <c r="D40" s="52" t="s">
+      <c r="D40" s="51" t="s">
         <v>66</v>
       </c>
-      <c r="E40" s="40" t="s">
+      <c r="E40" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="F40" s="39"/>
-      <c r="G40" s="39"/>
-      <c r="H40" s="39"/>
-      <c r="I40" s="39"/>
-      <c r="J40" s="39"/>
-      <c r="K40" s="39"/>
-      <c r="L40" s="39"/>
+      <c r="F40" s="38"/>
+      <c r="G40" s="38"/>
+      <c r="H40" s="38"/>
+      <c r="I40" s="38"/>
+      <c r="J40" s="38"/>
+      <c r="K40" s="38"/>
+      <c r="L40" s="38"/>
     </row>
     <row r="41" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="35" t="n">
+      <c r="A41" s="34" t="n">
         <v>1.84</v>
       </c>
-      <c r="B41" s="36" t="s">
+      <c r="B41" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C41" s="37" t="n">
+      <c r="C41" s="36" t="n">
         <v>50754</v>
       </c>
-      <c r="D41" s="52" t="s">
+      <c r="D41" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="E41" s="40" t="s">
+      <c r="E41" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="F41" s="39"/>
-      <c r="G41" s="39"/>
-      <c r="H41" s="39"/>
-      <c r="I41" s="39"/>
-      <c r="J41" s="39"/>
-      <c r="K41" s="39"/>
-      <c r="L41" s="39"/>
+      <c r="F41" s="38"/>
+      <c r="G41" s="38"/>
+      <c r="H41" s="38"/>
+      <c r="I41" s="38"/>
+      <c r="J41" s="38"/>
+      <c r="K41" s="38"/>
+      <c r="L41" s="38"/>
     </row>
     <row r="42" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="35" t="n">
+      <c r="A42" s="34" t="n">
         <v>1.84</v>
       </c>
-      <c r="B42" s="36" t="s">
+      <c r="B42" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C42" s="37" t="n">
+      <c r="C42" s="36" t="n">
         <v>50755</v>
       </c>
-      <c r="D42" s="43" t="s">
+      <c r="D42" s="42" t="s">
         <v>68</v>
       </c>
-      <c r="E42" s="40" t="s">
+      <c r="E42" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="F42" s="39"/>
-      <c r="G42" s="39"/>
-      <c r="H42" s="39"/>
-      <c r="I42" s="39"/>
-      <c r="J42" s="39"/>
-      <c r="K42" s="39"/>
-      <c r="L42" s="39"/>
+      <c r="F42" s="38"/>
+      <c r="G42" s="38"/>
+      <c r="H42" s="38"/>
+      <c r="I42" s="38"/>
+      <c r="J42" s="38"/>
+      <c r="K42" s="38"/>
+      <c r="L42" s="38"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="35"/>
-      <c r="B43" s="36"/>
-      <c r="C43" s="48"/>
-      <c r="D43" s="49" t="s">
+      <c r="A43" s="34"/>
+      <c r="B43" s="35"/>
+      <c r="C43" s="47"/>
+      <c r="D43" s="48" t="s">
         <v>69</v>
       </c>
-      <c r="E43" s="50"/>
-      <c r="F43" s="41"/>
-      <c r="G43" s="42"/>
-      <c r="H43" s="42"/>
-      <c r="I43" s="42"/>
-      <c r="J43" s="41"/>
-      <c r="K43" s="42"/>
-      <c r="L43" s="41"/>
+      <c r="E43" s="49"/>
+      <c r="F43" s="40"/>
+      <c r="G43" s="41"/>
+      <c r="H43" s="41"/>
+      <c r="I43" s="41"/>
+      <c r="J43" s="40"/>
+      <c r="K43" s="41"/>
+      <c r="L43" s="40"/>
     </row>
     <row r="44" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="35" t="n">
+      <c r="A44" s="34" t="n">
         <v>1.84</v>
       </c>
-      <c r="B44" s="36" t="s">
+      <c r="B44" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="C44" s="37" t="n">
+      <c r="C44" s="36" t="n">
         <v>50756</v>
       </c>
-      <c r="D44" s="40" t="s">
+      <c r="D44" s="39" t="s">
         <v>70</v>
       </c>
-      <c r="E44" s="40" t="s">
+      <c r="E44" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="F44" s="39"/>
-      <c r="G44" s="39"/>
-      <c r="H44" s="39"/>
-      <c r="I44" s="39"/>
-      <c r="J44" s="39"/>
-      <c r="K44" s="39"/>
-      <c r="L44" s="39"/>
+      <c r="F44" s="38"/>
+      <c r="G44" s="38"/>
+      <c r="H44" s="38"/>
+      <c r="I44" s="38"/>
+      <c r="J44" s="38"/>
+      <c r="K44" s="38"/>
+      <c r="L44" s="38"/>
     </row>
     <row r="45" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="35" t="n">
+      <c r="A45" s="34" t="n">
         <v>1.84</v>
       </c>
-      <c r="B45" s="36" t="s">
+      <c r="B45" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="C45" s="37" t="n">
+      <c r="C45" s="36" t="n">
         <v>50757</v>
       </c>
-      <c r="D45" s="40" t="s">
+      <c r="D45" s="39" t="s">
         <v>72</v>
       </c>
-      <c r="E45" s="40" t="s">
+      <c r="E45" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="F45" s="39"/>
-      <c r="G45" s="39"/>
-      <c r="H45" s="39"/>
-      <c r="I45" s="39"/>
-      <c r="J45" s="39"/>
-      <c r="K45" s="39"/>
-      <c r="L45" s="39"/>
+      <c r="F45" s="38"/>
+      <c r="G45" s="38"/>
+      <c r="H45" s="38"/>
+      <c r="I45" s="38"/>
+      <c r="J45" s="38"/>
+      <c r="K45" s="38"/>
+      <c r="L45" s="38"/>
     </row>
     <row r="46" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="35" t="n">
+      <c r="A46" s="34" t="n">
         <v>1.84</v>
       </c>
-      <c r="B46" s="36" t="s">
+      <c r="B46" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="C46" s="37" t="n">
+      <c r="C46" s="36" t="n">
         <v>50758</v>
       </c>
-      <c r="D46" s="40" t="s">
+      <c r="D46" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="E46" s="40" t="s">
+      <c r="E46" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="F46" s="39"/>
-      <c r="G46" s="39"/>
-      <c r="H46" s="39"/>
-      <c r="I46" s="39"/>
-      <c r="J46" s="39"/>
-      <c r="K46" s="39"/>
-      <c r="L46" s="39"/>
+      <c r="F46" s="38"/>
+      <c r="G46" s="38"/>
+      <c r="H46" s="38"/>
+      <c r="I46" s="38"/>
+      <c r="J46" s="38"/>
+      <c r="K46" s="38"/>
+      <c r="L46" s="38"/>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="35"/>
-      <c r="B47" s="36"/>
-      <c r="C47" s="48"/>
-      <c r="D47" s="49" t="s">
+      <c r="A47" s="34"/>
+      <c r="B47" s="35"/>
+      <c r="C47" s="47"/>
+      <c r="D47" s="48" t="s">
         <v>76</v>
       </c>
-      <c r="E47" s="50"/>
-      <c r="F47" s="41"/>
-      <c r="G47" s="42"/>
-      <c r="H47" s="42"/>
-      <c r="I47" s="42"/>
-      <c r="J47" s="41"/>
-      <c r="K47" s="42"/>
-      <c r="L47" s="41"/>
+      <c r="E47" s="49"/>
+      <c r="F47" s="40"/>
+      <c r="G47" s="41"/>
+      <c r="H47" s="41"/>
+      <c r="I47" s="41"/>
+      <c r="J47" s="40"/>
+      <c r="K47" s="41"/>
+      <c r="L47" s="40"/>
     </row>
     <row r="48" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="35" t="n">
+      <c r="A48" s="34" t="n">
         <v>2.3</v>
       </c>
-      <c r="B48" s="36" t="s">
+      <c r="B48" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="C48" s="37" t="n">
+      <c r="C48" s="36" t="n">
         <v>50759</v>
       </c>
-      <c r="D48" s="51" t="s">
+      <c r="D48" s="50" t="s">
         <v>77</v>
       </c>
-      <c r="E48" s="40" t="s">
+      <c r="E48" s="39" t="s">
         <v>78</v>
       </c>
-      <c r="F48" s="39"/>
-      <c r="G48" s="39"/>
-      <c r="H48" s="39"/>
-      <c r="I48" s="39"/>
-      <c r="J48" s="39"/>
-      <c r="K48" s="39"/>
-      <c r="L48" s="39"/>
+      <c r="F48" s="38"/>
+      <c r="G48" s="38"/>
+      <c r="H48" s="38"/>
+      <c r="I48" s="38"/>
+      <c r="J48" s="38"/>
+      <c r="K48" s="38"/>
+      <c r="L48" s="38"/>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="35"/>
-      <c r="B49" s="36"/>
-      <c r="C49" s="53"/>
-      <c r="D49" s="49" t="s">
+      <c r="A49" s="34"/>
+      <c r="B49" s="35"/>
+      <c r="C49" s="52"/>
+      <c r="D49" s="48" t="s">
         <v>79</v>
       </c>
-      <c r="E49" s="50"/>
-      <c r="F49" s="41"/>
-      <c r="G49" s="42"/>
-      <c r="H49" s="42"/>
-      <c r="I49" s="42"/>
-      <c r="J49" s="41"/>
-      <c r="K49" s="42"/>
-      <c r="L49" s="41"/>
+      <c r="E49" s="49"/>
+      <c r="F49" s="40"/>
+      <c r="G49" s="41"/>
+      <c r="H49" s="41"/>
+      <c r="I49" s="41"/>
+      <c r="J49" s="40"/>
+      <c r="K49" s="41"/>
+      <c r="L49" s="40"/>
     </row>
     <row r="50" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="35" t="n">
+      <c r="A50" s="34" t="n">
         <v>2.3</v>
       </c>
-      <c r="B50" s="36" t="s">
+      <c r="B50" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C50" s="37" t="n">
+      <c r="C50" s="36" t="n">
         <v>50760</v>
       </c>
-      <c r="D50" s="43" t="s">
+      <c r="D50" s="42" t="s">
         <v>80</v>
       </c>
-      <c r="E50" s="40" t="s">
+      <c r="E50" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="F50" s="39"/>
-      <c r="G50" s="39"/>
-      <c r="H50" s="39"/>
-      <c r="I50" s="39"/>
-      <c r="J50" s="39"/>
-      <c r="K50" s="39"/>
-      <c r="L50" s="39"/>
+      <c r="F50" s="38"/>
+      <c r="G50" s="38"/>
+      <c r="H50" s="38"/>
+      <c r="I50" s="38"/>
+      <c r="J50" s="38"/>
+      <c r="K50" s="38"/>
+      <c r="L50" s="38"/>
     </row>
     <row r="51" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="35" t="n">
+      <c r="A51" s="34" t="n">
         <v>2.3</v>
       </c>
-      <c r="B51" s="36" t="s">
+      <c r="B51" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C51" s="37" t="n">
+      <c r="C51" s="36" t="n">
         <v>50761</v>
       </c>
-      <c r="D51" s="43" t="s">
+      <c r="D51" s="42" t="s">
         <v>81</v>
       </c>
-      <c r="E51" s="40" t="s">
+      <c r="E51" s="39" t="s">
         <v>82</v>
       </c>
-      <c r="F51" s="39"/>
-      <c r="G51" s="39"/>
-      <c r="H51" s="39"/>
-      <c r="I51" s="39"/>
-      <c r="J51" s="39"/>
-      <c r="K51" s="39"/>
-      <c r="L51" s="39"/>
+      <c r="F51" s="38"/>
+      <c r="G51" s="38"/>
+      <c r="H51" s="38"/>
+      <c r="I51" s="38"/>
+      <c r="J51" s="38"/>
+      <c r="K51" s="38"/>
+      <c r="L51" s="38"/>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="35"/>
-      <c r="B52" s="36"/>
-      <c r="C52" s="48"/>
-      <c r="D52" s="49" t="s">
+      <c r="A52" s="34"/>
+      <c r="B52" s="35"/>
+      <c r="C52" s="47"/>
+      <c r="D52" s="48" t="s">
         <v>83</v>
       </c>
-      <c r="E52" s="50"/>
-      <c r="F52" s="41"/>
-      <c r="G52" s="42"/>
-      <c r="H52" s="42"/>
-      <c r="I52" s="42"/>
-      <c r="J52" s="41"/>
-      <c r="K52" s="42"/>
-      <c r="L52" s="41"/>
+      <c r="E52" s="49"/>
+      <c r="F52" s="40"/>
+      <c r="G52" s="41"/>
+      <c r="H52" s="41"/>
+      <c r="I52" s="41"/>
+      <c r="J52" s="40"/>
+      <c r="K52" s="41"/>
+      <c r="L52" s="40"/>
     </row>
     <row r="53" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="35" t="n">
+      <c r="A53" s="34" t="n">
         <v>2.3</v>
       </c>
-      <c r="B53" s="36" t="s">
+      <c r="B53" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C53" s="37" t="n">
+      <c r="C53" s="36" t="n">
         <v>50762</v>
       </c>
-      <c r="D53" s="43" t="s">
+      <c r="D53" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="E53" s="40" t="s">
+      <c r="E53" s="39" t="s">
         <v>85</v>
       </c>
-      <c r="F53" s="39"/>
-      <c r="G53" s="39"/>
-      <c r="H53" s="39"/>
-      <c r="I53" s="39"/>
-      <c r="J53" s="39"/>
-      <c r="K53" s="39"/>
-      <c r="L53" s="39"/>
+      <c r="F53" s="38"/>
+      <c r="G53" s="38"/>
+      <c r="H53" s="38"/>
+      <c r="I53" s="38"/>
+      <c r="J53" s="38"/>
+      <c r="K53" s="38"/>
+      <c r="L53" s="38"/>
     </row>
     <row r="54" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="35" t="n">
+      <c r="A54" s="34" t="n">
         <v>2.3</v>
       </c>
-      <c r="B54" s="36" t="s">
+      <c r="B54" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C54" s="37" t="n">
+      <c r="C54" s="36" t="n">
         <v>50763</v>
       </c>
-      <c r="D54" s="43" t="s">
+      <c r="D54" s="42" t="s">
         <v>86</v>
       </c>
-      <c r="E54" s="40" t="s">
+      <c r="E54" s="39" t="s">
         <v>87</v>
       </c>
-      <c r="F54" s="39"/>
-      <c r="G54" s="39"/>
-      <c r="H54" s="39"/>
-      <c r="I54" s="39"/>
-      <c r="J54" s="39"/>
-      <c r="K54" s="39"/>
-      <c r="L54" s="39"/>
+      <c r="F54" s="38"/>
+      <c r="G54" s="38"/>
+      <c r="H54" s="38"/>
+      <c r="I54" s="38"/>
+      <c r="J54" s="38"/>
+      <c r="K54" s="38"/>
+      <c r="L54" s="38"/>
     </row>
     <row r="55" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="35" t="n">
+      <c r="A55" s="34" t="n">
         <v>2.3</v>
       </c>
-      <c r="B55" s="36" t="s">
+      <c r="B55" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C55" s="37" t="n">
+      <c r="C55" s="36" t="n">
         <v>50764</v>
       </c>
-      <c r="D55" s="43" t="s">
+      <c r="D55" s="42" t="s">
         <v>88</v>
       </c>
-      <c r="E55" s="40" t="s">
+      <c r="E55" s="39" t="s">
         <v>87</v>
       </c>
-      <c r="F55" s="39"/>
-      <c r="G55" s="39"/>
-      <c r="H55" s="39"/>
-      <c r="I55" s="39"/>
-      <c r="J55" s="39"/>
-      <c r="K55" s="39"/>
-      <c r="L55" s="39"/>
+      <c r="F55" s="38"/>
+      <c r="G55" s="38"/>
+      <c r="H55" s="38"/>
+      <c r="I55" s="38"/>
+      <c r="J55" s="38"/>
+      <c r="K55" s="38"/>
+      <c r="L55" s="38"/>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="35"/>
-      <c r="B56" s="36"/>
-      <c r="C56" s="48"/>
-      <c r="D56" s="49" t="s">
+      <c r="A56" s="34"/>
+      <c r="B56" s="35"/>
+      <c r="C56" s="47"/>
+      <c r="D56" s="48" t="s">
         <v>89</v>
       </c>
-      <c r="E56" s="50"/>
-      <c r="F56" s="41"/>
-      <c r="G56" s="42"/>
-      <c r="H56" s="42"/>
-      <c r="I56" s="42"/>
-      <c r="J56" s="41"/>
-      <c r="K56" s="42"/>
-      <c r="L56" s="41"/>
+      <c r="E56" s="49"/>
+      <c r="F56" s="40"/>
+      <c r="G56" s="41"/>
+      <c r="H56" s="41"/>
+      <c r="I56" s="41"/>
+      <c r="J56" s="40"/>
+      <c r="K56" s="41"/>
+      <c r="L56" s="40"/>
     </row>
     <row r="57" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="35" t="n">
+      <c r="A57" s="34" t="n">
         <v>2.3</v>
       </c>
-      <c r="B57" s="36" t="s">
+      <c r="B57" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C57" s="37" t="n">
+      <c r="C57" s="36" t="n">
         <v>50765</v>
       </c>
-      <c r="D57" s="40" t="s">
+      <c r="D57" s="39" t="s">
         <v>90</v>
       </c>
-      <c r="E57" s="40" t="s">
+      <c r="E57" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="F57" s="39"/>
-      <c r="G57" s="39"/>
-      <c r="H57" s="39"/>
-      <c r="I57" s="39"/>
-      <c r="J57" s="39"/>
-      <c r="K57" s="39"/>
-      <c r="L57" s="39"/>
+      <c r="F57" s="38"/>
+      <c r="G57" s="38"/>
+      <c r="H57" s="38"/>
+      <c r="I57" s="38"/>
+      <c r="J57" s="38"/>
+      <c r="K57" s="38"/>
+      <c r="L57" s="38"/>
     </row>
     <row r="58" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="35" t="n">
+      <c r="A58" s="34" t="n">
         <v>2.3</v>
       </c>
-      <c r="B58" s="36" t="s">
+      <c r="B58" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C58" s="37" t="n">
+      <c r="C58" s="36" t="n">
         <v>50766</v>
       </c>
-      <c r="D58" s="54" t="s">
+      <c r="D58" s="53" t="s">
         <v>91</v>
       </c>
-      <c r="E58" s="40" t="s">
+      <c r="E58" s="39" t="s">
         <v>92</v>
       </c>
-      <c r="F58" s="39"/>
-      <c r="G58" s="39"/>
-      <c r="H58" s="39"/>
-      <c r="I58" s="39"/>
-      <c r="J58" s="39"/>
-      <c r="K58" s="39"/>
-      <c r="L58" s="39"/>
+      <c r="F58" s="38"/>
+      <c r="G58" s="38"/>
+      <c r="H58" s="38"/>
+      <c r="I58" s="38"/>
+      <c r="J58" s="38"/>
+      <c r="K58" s="38"/>
+      <c r="L58" s="38"/>
     </row>
     <row r="59" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="35" t="n">
+      <c r="A59" s="34" t="n">
         <v>2.3</v>
       </c>
-      <c r="B59" s="36" t="s">
+      <c r="B59" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C59" s="37" t="n">
+      <c r="C59" s="36" t="n">
         <v>50767</v>
       </c>
-      <c r="D59" s="43" t="s">
+      <c r="D59" s="42" t="s">
         <v>93</v>
       </c>
-      <c r="E59" s="40" t="s">
+      <c r="E59" s="39" t="s">
         <v>92</v>
       </c>
-      <c r="F59" s="39"/>
-      <c r="G59" s="39"/>
-      <c r="H59" s="39"/>
-      <c r="I59" s="39"/>
-      <c r="J59" s="39"/>
-      <c r="K59" s="39"/>
-      <c r="L59" s="39"/>
+      <c r="F59" s="38"/>
+      <c r="G59" s="38"/>
+      <c r="H59" s="38"/>
+      <c r="I59" s="38"/>
+      <c r="J59" s="38"/>
+      <c r="K59" s="38"/>
+      <c r="L59" s="38"/>
     </row>
     <row r="60" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="35" t="n">
+      <c r="A60" s="34" t="n">
         <v>2.3</v>
       </c>
-      <c r="B60" s="36" t="s">
+      <c r="B60" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C60" s="37" t="n">
+      <c r="C60" s="36" t="n">
         <v>50768</v>
       </c>
-      <c r="D60" s="43" t="s">
+      <c r="D60" s="42" t="s">
         <v>94</v>
       </c>
-      <c r="E60" s="40" t="s">
+      <c r="E60" s="39" t="s">
         <v>95</v>
       </c>
-      <c r="F60" s="39"/>
-      <c r="G60" s="39"/>
-      <c r="H60" s="39"/>
-      <c r="I60" s="39"/>
-      <c r="J60" s="39"/>
-      <c r="K60" s="39"/>
-      <c r="L60" s="39"/>
+      <c r="F60" s="38"/>
+      <c r="G60" s="38"/>
+      <c r="H60" s="38"/>
+      <c r="I60" s="38"/>
+      <c r="J60" s="38"/>
+      <c r="K60" s="38"/>
+      <c r="L60" s="38"/>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="35"/>
-      <c r="B61" s="36"/>
-      <c r="C61" s="48"/>
-      <c r="D61" s="49" t="s">
+      <c r="A61" s="34"/>
+      <c r="B61" s="35"/>
+      <c r="C61" s="47"/>
+      <c r="D61" s="48" t="s">
         <v>96</v>
       </c>
-      <c r="E61" s="50"/>
-      <c r="F61" s="41"/>
-      <c r="G61" s="42"/>
-      <c r="H61" s="42"/>
-      <c r="I61" s="42"/>
-      <c r="J61" s="41"/>
-      <c r="K61" s="42"/>
-      <c r="L61" s="41"/>
+      <c r="E61" s="49"/>
+      <c r="F61" s="40"/>
+      <c r="G61" s="41"/>
+      <c r="H61" s="41"/>
+      <c r="I61" s="41"/>
+      <c r="J61" s="40"/>
+      <c r="K61" s="41"/>
+      <c r="L61" s="40"/>
     </row>
     <row r="62" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="35" t="n">
+      <c r="A62" s="34" t="n">
         <v>2.3</v>
       </c>
-      <c r="B62" s="36" t="s">
+      <c r="B62" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="C62" s="44" t="n">
+      <c r="C62" s="43" t="n">
         <v>50817</v>
       </c>
-      <c r="D62" s="46" t="s">
+      <c r="D62" s="45" t="s">
         <v>97</v>
       </c>
-      <c r="E62" s="40" t="s">
+      <c r="E62" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="F62" s="39"/>
-      <c r="G62" s="39"/>
-      <c r="H62" s="39"/>
-      <c r="I62" s="39"/>
-      <c r="J62" s="39"/>
-      <c r="K62" s="39"/>
-      <c r="L62" s="39"/>
+      <c r="F62" s="38"/>
+      <c r="G62" s="38"/>
+      <c r="H62" s="38"/>
+      <c r="I62" s="38"/>
+      <c r="J62" s="38"/>
+      <c r="K62" s="38"/>
+      <c r="L62" s="38"/>
     </row>
     <row r="63" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="35" t="n">
+      <c r="A63" s="34" t="n">
         <v>2.3</v>
       </c>
-      <c r="B63" s="36" t="s">
+      <c r="B63" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C63" s="37" t="n">
+      <c r="C63" s="36" t="n">
         <v>50770</v>
       </c>
-      <c r="D63" s="47" t="s">
+      <c r="D63" s="46" t="s">
         <v>98</v>
       </c>
-      <c r="E63" s="40" t="s">
+      <c r="E63" s="39" t="s">
         <v>99</v>
       </c>
-      <c r="F63" s="39"/>
-      <c r="G63" s="39"/>
-      <c r="H63" s="39"/>
-      <c r="I63" s="39"/>
-      <c r="J63" s="39"/>
-      <c r="K63" s="39"/>
-      <c r="L63" s="39"/>
+      <c r="F63" s="38"/>
+      <c r="G63" s="38"/>
+      <c r="H63" s="38"/>
+      <c r="I63" s="38"/>
+      <c r="J63" s="38"/>
+      <c r="K63" s="38"/>
+      <c r="L63" s="38"/>
     </row>
     <row r="64" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="35" t="n">
+      <c r="A64" s="34" t="n">
         <v>2.3</v>
       </c>
-      <c r="B64" s="36" t="s">
+      <c r="B64" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C64" s="37" t="n">
+      <c r="C64" s="36" t="n">
         <v>50771</v>
       </c>
-      <c r="D64" s="43" t="s">
+      <c r="D64" s="42" t="s">
         <v>100</v>
       </c>
-      <c r="E64" s="40" t="s">
+      <c r="E64" s="39" t="s">
         <v>101</v>
       </c>
-      <c r="F64" s="39"/>
-      <c r="G64" s="39"/>
-      <c r="H64" s="39"/>
-      <c r="I64" s="39"/>
-      <c r="J64" s="39"/>
-      <c r="K64" s="39"/>
-      <c r="L64" s="39"/>
+      <c r="F64" s="38"/>
+      <c r="G64" s="38"/>
+      <c r="H64" s="38"/>
+      <c r="I64" s="38"/>
+      <c r="J64" s="38"/>
+      <c r="K64" s="38"/>
+      <c r="L64" s="38"/>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="35"/>
-      <c r="B65" s="36"/>
-      <c r="C65" s="48"/>
-      <c r="D65" s="49" t="s">
+      <c r="A65" s="34"/>
+      <c r="B65" s="35"/>
+      <c r="C65" s="47"/>
+      <c r="D65" s="48" t="s">
         <v>102</v>
       </c>
-      <c r="E65" s="50"/>
-      <c r="F65" s="41"/>
-      <c r="G65" s="42"/>
-      <c r="H65" s="42"/>
-      <c r="I65" s="42"/>
-      <c r="J65" s="41"/>
-      <c r="K65" s="42"/>
-      <c r="L65" s="41"/>
+      <c r="E65" s="49"/>
+      <c r="F65" s="40"/>
+      <c r="G65" s="41"/>
+      <c r="H65" s="41"/>
+      <c r="I65" s="41"/>
+      <c r="J65" s="40"/>
+      <c r="K65" s="41"/>
+      <c r="L65" s="40"/>
     </row>
     <row r="66" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="35" t="n">
+      <c r="A66" s="34" t="n">
         <v>1.84</v>
       </c>
-      <c r="B66" s="36" t="s">
+      <c r="B66" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="C66" s="37" t="n">
+      <c r="C66" s="36" t="n">
         <v>50772</v>
       </c>
-      <c r="D66" s="40" t="s">
+      <c r="D66" s="39" t="s">
         <v>103</v>
       </c>
-      <c r="E66" s="40" t="s">
+      <c r="E66" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="F66" s="39"/>
-      <c r="G66" s="39"/>
-      <c r="H66" s="39"/>
-      <c r="I66" s="39"/>
-      <c r="J66" s="39"/>
-      <c r="K66" s="39"/>
-      <c r="L66" s="39"/>
+      <c r="F66" s="38"/>
+      <c r="G66" s="38"/>
+      <c r="H66" s="38"/>
+      <c r="I66" s="38"/>
+      <c r="J66" s="38"/>
+      <c r="K66" s="38"/>
+      <c r="L66" s="38"/>
     </row>
     <row r="67" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="35" t="n">
+      <c r="A67" s="34" t="n">
         <v>2.3</v>
       </c>
-      <c r="B67" s="36" t="s">
+      <c r="B67" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="C67" s="37" t="n">
+      <c r="C67" s="36" t="n">
         <v>50773</v>
       </c>
-      <c r="D67" s="40" t="s">
+      <c r="D67" s="39" t="s">
         <v>105</v>
       </c>
-      <c r="E67" s="40" t="s">
+      <c r="E67" s="39" t="s">
         <v>106</v>
       </c>
-      <c r="F67" s="39"/>
-      <c r="G67" s="39"/>
-      <c r="H67" s="39"/>
-      <c r="I67" s="39"/>
-      <c r="J67" s="39"/>
-      <c r="K67" s="39"/>
-      <c r="L67" s="39"/>
+      <c r="F67" s="38"/>
+      <c r="G67" s="38"/>
+      <c r="H67" s="38"/>
+      <c r="I67" s="38"/>
+      <c r="J67" s="38"/>
+      <c r="K67" s="38"/>
+      <c r="L67" s="38"/>
     </row>
     <row r="68" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="35" t="n">
+      <c r="A68" s="34" t="n">
         <v>2.3</v>
       </c>
-      <c r="B68" s="36" t="s">
+      <c r="B68" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="C68" s="37" t="n">
+      <c r="C68" s="36" t="n">
         <v>50774</v>
       </c>
-      <c r="D68" s="40" t="s">
+      <c r="D68" s="39" t="s">
         <v>107</v>
       </c>
-      <c r="E68" s="40" t="s">
+      <c r="E68" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="F68" s="39"/>
-      <c r="G68" s="39"/>
-      <c r="H68" s="39"/>
-      <c r="I68" s="39"/>
-      <c r="J68" s="39"/>
-      <c r="K68" s="39"/>
-      <c r="L68" s="39"/>
+      <c r="F68" s="38"/>
+      <c r="G68" s="38"/>
+      <c r="H68" s="38"/>
+      <c r="I68" s="38"/>
+      <c r="J68" s="38"/>
+      <c r="K68" s="38"/>
+      <c r="L68" s="38"/>
     </row>
     <row r="69" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="35" t="n">
+      <c r="A69" s="34" t="n">
         <v>1.84</v>
       </c>
-      <c r="B69" s="36" t="s">
+      <c r="B69" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C69" s="37" t="n">
+      <c r="C69" s="36" t="n">
         <v>50775</v>
       </c>
-      <c r="D69" s="55" t="s">
+      <c r="D69" s="54" t="s">
         <v>109</v>
       </c>
-      <c r="E69" s="40" t="s">
+      <c r="E69" s="39" t="s">
         <v>110</v>
       </c>
-      <c r="F69" s="39"/>
-      <c r="G69" s="39"/>
-      <c r="H69" s="39"/>
-      <c r="I69" s="39"/>
-      <c r="J69" s="39"/>
-      <c r="K69" s="39"/>
-      <c r="L69" s="39"/>
+      <c r="F69" s="38"/>
+      <c r="G69" s="38"/>
+      <c r="H69" s="38"/>
+      <c r="I69" s="38"/>
+      <c r="J69" s="38"/>
+      <c r="K69" s="38"/>
+      <c r="L69" s="38"/>
     </row>
     <row r="70" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="35" t="n">
+      <c r="A70" s="34" t="n">
         <v>1.84</v>
       </c>
-      <c r="B70" s="36" t="s">
+      <c r="B70" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C70" s="37" t="n">
+      <c r="C70" s="36" t="n">
         <v>50776</v>
       </c>
-      <c r="D70" s="43" t="s">
+      <c r="D70" s="42" t="s">
         <v>111</v>
       </c>
-      <c r="E70" s="40" t="s">
+      <c r="E70" s="39" t="s">
         <v>112</v>
       </c>
-      <c r="F70" s="41"/>
-      <c r="G70" s="42"/>
-      <c r="H70" s="42"/>
-      <c r="I70" s="42"/>
-      <c r="J70" s="41"/>
-      <c r="K70" s="42"/>
-      <c r="L70" s="41"/>
+      <c r="F70" s="40"/>
+      <c r="G70" s="41"/>
+      <c r="H70" s="41"/>
+      <c r="I70" s="41"/>
+      <c r="J70" s="40"/>
+      <c r="K70" s="41"/>
+      <c r="L70" s="40"/>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="35"/>
-      <c r="B71" s="36"/>
-      <c r="C71" s="48"/>
-      <c r="D71" s="49" t="s">
+      <c r="A71" s="34"/>
+      <c r="B71" s="35"/>
+      <c r="C71" s="47"/>
+      <c r="D71" s="48" t="s">
         <v>113</v>
       </c>
-      <c r="E71" s="50"/>
-      <c r="F71" s="41"/>
-      <c r="G71" s="42"/>
-      <c r="H71" s="42"/>
-      <c r="I71" s="42"/>
-      <c r="J71" s="41"/>
-      <c r="K71" s="42"/>
-      <c r="L71" s="41"/>
+      <c r="E71" s="49"/>
+      <c r="F71" s="40"/>
+      <c r="G71" s="41"/>
+      <c r="H71" s="41"/>
+      <c r="I71" s="41"/>
+      <c r="J71" s="40"/>
+      <c r="K71" s="41"/>
+      <c r="L71" s="40"/>
     </row>
     <row r="72" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="35" t="n">
+      <c r="A72" s="34" t="n">
         <v>2.3</v>
       </c>
-      <c r="B72" s="36" t="s">
+      <c r="B72" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="C72" s="37" t="n">
+      <c r="C72" s="36" t="n">
         <v>50777</v>
       </c>
-      <c r="D72" s="56" t="s">
+      <c r="D72" s="55" t="s">
         <v>114</v>
       </c>
-      <c r="E72" s="40" t="s">
+      <c r="E72" s="39" t="s">
         <v>115</v>
       </c>
-      <c r="F72" s="39"/>
-      <c r="G72" s="39"/>
-      <c r="H72" s="39"/>
-      <c r="I72" s="39"/>
-      <c r="J72" s="39"/>
-      <c r="K72" s="39"/>
-      <c r="L72" s="39"/>
+      <c r="F72" s="38"/>
+      <c r="G72" s="38"/>
+      <c r="H72" s="38"/>
+      <c r="I72" s="38"/>
+      <c r="J72" s="38"/>
+      <c r="K72" s="38"/>
+      <c r="L72" s="38"/>
     </row>
     <row r="73" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="35" t="n">
+      <c r="A73" s="34" t="n">
         <v>2.3</v>
       </c>
-      <c r="B73" s="36" t="s">
+      <c r="B73" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="C73" s="37" t="n">
+      <c r="C73" s="36" t="n">
         <v>50778</v>
       </c>
-      <c r="D73" s="40" t="s">
+      <c r="D73" s="39" t="s">
         <v>116</v>
       </c>
-      <c r="E73" s="40" t="s">
+      <c r="E73" s="39" t="s">
         <v>110</v>
       </c>
-      <c r="F73" s="39"/>
-      <c r="G73" s="39"/>
-      <c r="H73" s="39"/>
-      <c r="I73" s="39"/>
-      <c r="J73" s="39"/>
-      <c r="K73" s="39"/>
-      <c r="L73" s="39"/>
+      <c r="F73" s="38"/>
+      <c r="G73" s="38"/>
+      <c r="H73" s="38"/>
+      <c r="I73" s="38"/>
+      <c r="J73" s="38"/>
+      <c r="K73" s="38"/>
+      <c r="L73" s="38"/>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="35"/>
-      <c r="B74" s="36"/>
-      <c r="C74" s="48"/>
-      <c r="D74" s="49" t="s">
+      <c r="A74" s="34"/>
+      <c r="B74" s="35"/>
+      <c r="C74" s="47"/>
+      <c r="D74" s="48" t="s">
         <v>117</v>
       </c>
-      <c r="E74" s="50"/>
-      <c r="F74" s="41"/>
-      <c r="G74" s="42"/>
-      <c r="H74" s="42"/>
-      <c r="I74" s="42"/>
-      <c r="J74" s="41"/>
-      <c r="K74" s="42"/>
-      <c r="L74" s="41"/>
+      <c r="E74" s="49"/>
+      <c r="F74" s="40"/>
+      <c r="G74" s="41"/>
+      <c r="H74" s="41"/>
+      <c r="I74" s="41"/>
+      <c r="J74" s="40"/>
+      <c r="K74" s="41"/>
+      <c r="L74" s="40"/>
     </row>
     <row r="75" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="35" t="n">
+      <c r="A75" s="34" t="n">
         <v>2.3</v>
       </c>
-      <c r="B75" s="36" t="s">
+      <c r="B75" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C75" s="37" t="n">
+      <c r="C75" s="36" t="n">
         <v>50779</v>
       </c>
-      <c r="D75" s="43" t="s">
+      <c r="D75" s="42" t="s">
         <v>118</v>
       </c>
-      <c r="E75" s="40" t="s">
+      <c r="E75" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="F75" s="57"/>
-      <c r="G75" s="57"/>
-      <c r="H75" s="57"/>
-      <c r="I75" s="57"/>
-      <c r="J75" s="57"/>
-      <c r="K75" s="57"/>
-      <c r="L75" s="57"/>
+      <c r="F75" s="38"/>
+      <c r="G75" s="38"/>
+      <c r="H75" s="38"/>
+      <c r="I75" s="38"/>
+      <c r="J75" s="38"/>
+      <c r="K75" s="38"/>
+      <c r="L75" s="38"/>
     </row>
     <row r="76" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="35" t="n">
+      <c r="A76" s="34" t="n">
         <v>2.3</v>
       </c>
-      <c r="B76" s="36" t="s">
+      <c r="B76" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C76" s="37" t="n">
+      <c r="C76" s="36" t="n">
         <v>50780</v>
       </c>
-      <c r="D76" s="43" t="s">
+      <c r="D76" s="42" t="s">
         <v>119</v>
       </c>
-      <c r="E76" s="40" t="s">
+      <c r="E76" s="39" t="s">
         <v>112</v>
       </c>
-      <c r="F76" s="57"/>
-      <c r="G76" s="57"/>
-      <c r="H76" s="57"/>
-      <c r="I76" s="57"/>
-      <c r="J76" s="57"/>
-      <c r="K76" s="57"/>
-      <c r="L76" s="57"/>
+      <c r="F76" s="38"/>
+      <c r="G76" s="38"/>
+      <c r="H76" s="38"/>
+      <c r="I76" s="38"/>
+      <c r="J76" s="38"/>
+      <c r="K76" s="38"/>
+      <c r="L76" s="38"/>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="35"/>
-      <c r="B77" s="36"/>
-      <c r="C77" s="48"/>
-      <c r="D77" s="49" t="s">
+      <c r="A77" s="34"/>
+      <c r="B77" s="35"/>
+      <c r="C77" s="47"/>
+      <c r="D77" s="48" t="s">
         <v>120</v>
       </c>
-      <c r="E77" s="50"/>
-      <c r="F77" s="41"/>
-      <c r="G77" s="42"/>
-      <c r="H77" s="42"/>
-      <c r="I77" s="42"/>
-      <c r="J77" s="41"/>
-      <c r="K77" s="42"/>
-      <c r="L77" s="41"/>
+      <c r="E77" s="49"/>
+      <c r="F77" s="40"/>
+      <c r="G77" s="41"/>
+      <c r="H77" s="41"/>
+      <c r="I77" s="41"/>
+      <c r="J77" s="40"/>
+      <c r="K77" s="41"/>
+      <c r="L77" s="40"/>
     </row>
     <row r="78" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="35" t="n">
+      <c r="A78" s="34" t="n">
         <v>1.61</v>
       </c>
-      <c r="B78" s="36" t="s">
+      <c r="B78" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C78" s="37" t="n">
+      <c r="C78" s="36" t="n">
         <v>50781</v>
       </c>
-      <c r="D78" s="43" t="s">
+      <c r="D78" s="42" t="s">
         <v>121</v>
       </c>
-      <c r="E78" s="40" t="s">
+      <c r="E78" s="39" t="s">
         <v>122</v>
       </c>
-      <c r="F78" s="57"/>
-      <c r="G78" s="57"/>
-      <c r="H78" s="57"/>
-      <c r="I78" s="57"/>
-      <c r="J78" s="57"/>
-      <c r="K78" s="57"/>
-      <c r="L78" s="57"/>
+      <c r="F78" s="38"/>
+      <c r="G78" s="38"/>
+      <c r="H78" s="38"/>
+      <c r="I78" s="38"/>
+      <c r="J78" s="38"/>
+      <c r="K78" s="38"/>
+      <c r="L78" s="38"/>
     </row>
     <row r="79" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="35" t="n">
+      <c r="A79" s="34" t="n">
         <v>1.61</v>
       </c>
-      <c r="B79" s="36" t="s">
+      <c r="B79" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C79" s="37" t="n">
+      <c r="C79" s="36" t="n">
         <v>50782</v>
       </c>
-      <c r="D79" s="40" t="s">
+      <c r="D79" s="39" t="s">
         <v>123</v>
       </c>
-      <c r="E79" s="40" t="s">
+      <c r="E79" s="39" t="s">
         <v>124</v>
       </c>
-      <c r="F79" s="57"/>
-      <c r="G79" s="57"/>
-      <c r="H79" s="57"/>
-      <c r="I79" s="57"/>
-      <c r="J79" s="57"/>
-      <c r="K79" s="57"/>
-      <c r="L79" s="57"/>
+      <c r="F79" s="38"/>
+      <c r="G79" s="38"/>
+      <c r="H79" s="38"/>
+      <c r="I79" s="38"/>
+      <c r="J79" s="38"/>
+      <c r="K79" s="38"/>
+      <c r="L79" s="38"/>
     </row>
     <row r="80" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="35" t="n">
+      <c r="A80" s="34" t="n">
         <v>1.61</v>
       </c>
-      <c r="B80" s="36" t="s">
+      <c r="B80" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C80" s="37" t="n">
+      <c r="C80" s="36" t="n">
         <v>50783</v>
       </c>
-      <c r="D80" s="43" t="s">
+      <c r="D80" s="42" t="s">
         <v>125</v>
       </c>
-      <c r="E80" s="40" t="s">
+      <c r="E80" s="39" t="s">
         <v>126</v>
       </c>
-      <c r="F80" s="57"/>
-      <c r="G80" s="57"/>
-      <c r="H80" s="57"/>
-      <c r="I80" s="57"/>
-      <c r="J80" s="57"/>
-      <c r="K80" s="57"/>
-      <c r="L80" s="57"/>
+      <c r="F80" s="38"/>
+      <c r="G80" s="38"/>
+      <c r="H80" s="38"/>
+      <c r="I80" s="38"/>
+      <c r="J80" s="38"/>
+      <c r="K80" s="38"/>
+      <c r="L80" s="38"/>
     </row>
     <row r="81" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="35" t="n">
+      <c r="A81" s="34" t="n">
         <v>1.84</v>
       </c>
-      <c r="B81" s="36" t="s">
+      <c r="B81" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C81" s="37" t="n">
+      <c r="C81" s="36" t="n">
         <v>50784</v>
       </c>
-      <c r="D81" s="40" t="s">
+      <c r="D81" s="39" t="s">
         <v>127</v>
       </c>
-      <c r="E81" s="40" t="s">
+      <c r="E81" s="39" t="s">
         <v>124</v>
       </c>
-      <c r="F81" s="57"/>
-      <c r="G81" s="57"/>
-      <c r="H81" s="57"/>
-      <c r="I81" s="57"/>
-      <c r="J81" s="57"/>
-      <c r="K81" s="57"/>
-      <c r="L81" s="57"/>
+      <c r="F81" s="38"/>
+      <c r="G81" s="38"/>
+      <c r="H81" s="38"/>
+      <c r="I81" s="38"/>
+      <c r="J81" s="38"/>
+      <c r="K81" s="38"/>
+      <c r="L81" s="38"/>
     </row>
     <row r="82" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="35" t="n">
+      <c r="A82" s="34" t="n">
         <v>1.84</v>
       </c>
-      <c r="B82" s="36" t="s">
+      <c r="B82" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C82" s="37" t="n">
+      <c r="C82" s="36" t="n">
         <v>50785</v>
       </c>
-      <c r="D82" s="43" t="s">
+      <c r="D82" s="42" t="s">
         <v>128</v>
       </c>
-      <c r="E82" s="40" t="s">
+      <c r="E82" s="39" t="s">
         <v>129</v>
       </c>
-      <c r="F82" s="57"/>
-      <c r="G82" s="57"/>
-      <c r="H82" s="57"/>
-      <c r="I82" s="57"/>
-      <c r="J82" s="57"/>
-      <c r="K82" s="57"/>
-      <c r="L82" s="57"/>
+      <c r="F82" s="38"/>
+      <c r="G82" s="38"/>
+      <c r="H82" s="38"/>
+      <c r="I82" s="38"/>
+      <c r="J82" s="38"/>
+      <c r="K82" s="38"/>
+      <c r="L82" s="38"/>
     </row>
     <row r="83" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="35" t="n">
+      <c r="A83" s="34" t="n">
         <v>2.06</v>
       </c>
-      <c r="B83" s="36" t="s">
+      <c r="B83" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C83" s="37" t="n">
+      <c r="C83" s="36" t="n">
         <v>50786</v>
       </c>
-      <c r="D83" s="40" t="s">
+      <c r="D83" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="E83" s="40" t="s">
+      <c r="E83" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="F83" s="41"/>
-      <c r="G83" s="42"/>
-      <c r="H83" s="42"/>
-      <c r="I83" s="42"/>
-      <c r="J83" s="41"/>
-      <c r="K83" s="42"/>
-      <c r="L83" s="41"/>
+      <c r="F83" s="40"/>
+      <c r="G83" s="41"/>
+      <c r="H83" s="41"/>
+      <c r="I83" s="41"/>
+      <c r="J83" s="40"/>
+      <c r="K83" s="41"/>
+      <c r="L83" s="40"/>
     </row>
     <row r="84" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="35" t="n">
+      <c r="A84" s="34" t="n">
         <v>2.06</v>
       </c>
-      <c r="B84" s="36" t="s">
+      <c r="B84" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C84" s="37" t="n">
+      <c r="C84" s="36" t="n">
         <v>50787</v>
       </c>
-      <c r="D84" s="43" t="s">
+      <c r="D84" s="42" t="s">
         <v>131</v>
       </c>
-      <c r="E84" s="40" t="s">
+      <c r="E84" s="39" t="s">
         <v>78</v>
       </c>
-      <c r="F84" s="57"/>
-      <c r="G84" s="57"/>
-      <c r="H84" s="57"/>
-      <c r="I84" s="57"/>
-      <c r="J84" s="57"/>
-      <c r="K84" s="57"/>
-      <c r="L84" s="57"/>
+      <c r="F84" s="38"/>
+      <c r="G84" s="38"/>
+      <c r="H84" s="38"/>
+      <c r="I84" s="38"/>
+      <c r="J84" s="38"/>
+      <c r="K84" s="38"/>
+      <c r="L84" s="38"/>
     </row>
     <row r="85" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="35" t="n">
+      <c r="A85" s="34" t="n">
         <v>3.44</v>
       </c>
-      <c r="B85" s="36" t="s">
+      <c r="B85" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C85" s="37" t="n">
+      <c r="C85" s="36" t="n">
         <v>50788</v>
       </c>
-      <c r="D85" s="40" t="s">
+      <c r="D85" s="39" t="s">
         <v>132</v>
       </c>
-      <c r="E85" s="40" t="s">
+      <c r="E85" s="39" t="s">
         <v>133</v>
       </c>
-      <c r="F85" s="57"/>
-      <c r="G85" s="57"/>
-      <c r="H85" s="57"/>
-      <c r="I85" s="57"/>
-      <c r="J85" s="57"/>
-      <c r="K85" s="57"/>
-      <c r="L85" s="57"/>
+      <c r="F85" s="38"/>
+      <c r="G85" s="38"/>
+      <c r="H85" s="38"/>
+      <c r="I85" s="38"/>
+      <c r="J85" s="38"/>
+      <c r="K85" s="38"/>
+      <c r="L85" s="38"/>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="35"/>
-      <c r="B86" s="36"/>
-      <c r="C86" s="48"/>
-      <c r="D86" s="49" t="s">
+      <c r="A86" s="34"/>
+      <c r="B86" s="35"/>
+      <c r="C86" s="47"/>
+      <c r="D86" s="48" t="s">
         <v>134</v>
       </c>
-      <c r="E86" s="50"/>
-      <c r="F86" s="41"/>
-      <c r="G86" s="42"/>
-      <c r="H86" s="42"/>
-      <c r="I86" s="42"/>
-      <c r="J86" s="41"/>
-      <c r="K86" s="42"/>
-      <c r="L86" s="41"/>
+      <c r="E86" s="49"/>
+      <c r="F86" s="40"/>
+      <c r="G86" s="41"/>
+      <c r="H86" s="41"/>
+      <c r="I86" s="41"/>
+      <c r="J86" s="40"/>
+      <c r="K86" s="41"/>
+      <c r="L86" s="40"/>
     </row>
     <row r="87" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="35" t="n">
+      <c r="A87" s="34" t="n">
         <v>1.71</v>
       </c>
-      <c r="B87" s="36" t="s">
+      <c r="B87" s="35" t="s">
         <v>135</v>
       </c>
-      <c r="C87" s="58" t="n">
+      <c r="C87" s="56" t="n">
         <v>50807</v>
       </c>
-      <c r="D87" s="43" t="s">
+      <c r="D87" s="42" t="s">
         <v>136</v>
       </c>
-      <c r="E87" s="40" t="s">
+      <c r="E87" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="F87" s="57"/>
-      <c r="G87" s="57"/>
-      <c r="H87" s="57"/>
-      <c r="I87" s="57"/>
-      <c r="J87" s="57"/>
-      <c r="K87" s="57"/>
-      <c r="L87" s="57"/>
+      <c r="F87" s="38"/>
+      <c r="G87" s="38"/>
+      <c r="H87" s="38"/>
+      <c r="I87" s="38"/>
+      <c r="J87" s="38"/>
+      <c r="K87" s="38"/>
+      <c r="L87" s="38"/>
     </row>
     <row r="88" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="35" t="n">
+      <c r="A88" s="34" t="n">
         <v>1.71</v>
       </c>
-      <c r="B88" s="36" t="s">
+      <c r="B88" s="35" t="s">
         <v>135</v>
       </c>
-      <c r="C88" s="58" t="n">
+      <c r="C88" s="56" t="n">
         <v>50808</v>
       </c>
-      <c r="D88" s="40" t="s">
+      <c r="D88" s="39" t="s">
         <v>137</v>
       </c>
-      <c r="E88" s="40" t="s">
+      <c r="E88" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="F88" s="57"/>
-      <c r="G88" s="57"/>
-      <c r="H88" s="57"/>
-      <c r="I88" s="57"/>
-      <c r="J88" s="57"/>
-      <c r="K88" s="57"/>
-      <c r="L88" s="57"/>
+      <c r="F88" s="38"/>
+      <c r="G88" s="38"/>
+      <c r="H88" s="38"/>
+      <c r="I88" s="38"/>
+      <c r="J88" s="38"/>
+      <c r="K88" s="38"/>
+      <c r="L88" s="38"/>
     </row>
     <row r="89" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="35" t="n">
+      <c r="A89" s="34" t="n">
         <v>1.71</v>
       </c>
-      <c r="B89" s="36" t="s">
+      <c r="B89" s="35" t="s">
         <v>135</v>
       </c>
-      <c r="C89" s="58" t="n">
+      <c r="C89" s="56" t="n">
         <v>50809</v>
       </c>
-      <c r="D89" s="43" t="s">
+      <c r="D89" s="42" t="s">
         <v>138</v>
       </c>
-      <c r="E89" s="40" t="s">
+      <c r="E89" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="F89" s="57"/>
-      <c r="G89" s="57"/>
-      <c r="H89" s="57"/>
-      <c r="I89" s="57"/>
-      <c r="J89" s="57"/>
-      <c r="K89" s="57"/>
-      <c r="L89" s="57"/>
+      <c r="F89" s="38"/>
+      <c r="G89" s="38"/>
+      <c r="H89" s="38"/>
+      <c r="I89" s="38"/>
+      <c r="J89" s="38"/>
+      <c r="K89" s="38"/>
+      <c r="L89" s="38"/>
     </row>
     <row r="90" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="35" t="n">
+      <c r="A90" s="34" t="n">
         <v>1.71</v>
       </c>
-      <c r="B90" s="36" t="s">
+      <c r="B90" s="35" t="s">
         <v>135</v>
       </c>
-      <c r="C90" s="58" t="n">
+      <c r="C90" s="56" t="n">
         <v>50810</v>
       </c>
-      <c r="D90" s="40" t="s">
+      <c r="D90" s="39" t="s">
         <v>139</v>
       </c>
-      <c r="E90" s="40" t="s">
+      <c r="E90" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="F90" s="41"/>
-      <c r="G90" s="42"/>
-      <c r="H90" s="42"/>
-      <c r="I90" s="42"/>
-      <c r="J90" s="41"/>
-      <c r="K90" s="42"/>
-      <c r="L90" s="41"/>
+      <c r="F90" s="40"/>
+      <c r="G90" s="41"/>
+      <c r="H90" s="41"/>
+      <c r="I90" s="41"/>
+      <c r="J90" s="40"/>
+      <c r="K90" s="41"/>
+      <c r="L90" s="40"/>
     </row>
     <row r="91" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="35" t="n">
+      <c r="A91" s="34" t="n">
         <v>2.18</v>
       </c>
-      <c r="B91" s="36" t="s">
+      <c r="B91" s="35" t="s">
         <v>135</v>
       </c>
-      <c r="C91" s="58" t="n">
+      <c r="C91" s="56" t="n">
         <v>50811</v>
       </c>
-      <c r="D91" s="43" t="s">
+      <c r="D91" s="42" t="s">
         <v>140</v>
       </c>
-      <c r="E91" s="40" t="s">
+      <c r="E91" s="39" t="s">
         <v>141</v>
       </c>
-      <c r="F91" s="39"/>
-      <c r="G91" s="39"/>
-      <c r="H91" s="39"/>
-      <c r="I91" s="39"/>
-      <c r="J91" s="39"/>
-      <c r="K91" s="39"/>
-      <c r="L91" s="39"/>
+      <c r="F91" s="38"/>
+      <c r="G91" s="38"/>
+      <c r="H91" s="38"/>
+      <c r="I91" s="38"/>
+      <c r="J91" s="38"/>
+      <c r="K91" s="38"/>
+      <c r="L91" s="38"/>
     </row>
     <row r="92" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="35" t="n">
+      <c r="A92" s="34" t="n">
         <v>2.67</v>
       </c>
-      <c r="B92" s="36" t="s">
+      <c r="B92" s="35" t="s">
         <v>135</v>
       </c>
-      <c r="C92" s="58" t="n">
+      <c r="C92" s="56" t="n">
         <v>50812</v>
       </c>
-      <c r="D92" s="40" t="s">
+      <c r="D92" s="39" t="s">
         <v>142</v>
       </c>
-      <c r="E92" s="40" t="s">
+      <c r="E92" s="39" t="s">
         <v>143</v>
       </c>
-      <c r="F92" s="39"/>
-      <c r="G92" s="39"/>
-      <c r="H92" s="39"/>
-      <c r="I92" s="39"/>
-      <c r="J92" s="39"/>
-      <c r="K92" s="39"/>
-      <c r="L92" s="39"/>
+      <c r="F92" s="38"/>
+      <c r="G92" s="38"/>
+      <c r="H92" s="38"/>
+      <c r="I92" s="38"/>
+      <c r="J92" s="38"/>
+      <c r="K92" s="38"/>
+      <c r="L92" s="38"/>
     </row>
     <row r="93" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="35" t="n">
+      <c r="A93" s="34" t="n">
         <v>2.67</v>
       </c>
-      <c r="B93" s="36" t="s">
+      <c r="B93" s="35" t="s">
         <v>135</v>
       </c>
-      <c r="C93" s="58" t="n">
+      <c r="C93" s="56" t="n">
         <v>50813</v>
       </c>
-      <c r="D93" s="43" t="s">
+      <c r="D93" s="42" t="s">
         <v>144</v>
       </c>
-      <c r="E93" s="40" t="s">
+      <c r="E93" s="39" t="s">
         <v>143</v>
       </c>
-      <c r="F93" s="39"/>
-      <c r="G93" s="39"/>
-      <c r="H93" s="39"/>
-      <c r="I93" s="39"/>
-      <c r="J93" s="39"/>
-      <c r="K93" s="39"/>
-      <c r="L93" s="39"/>
+      <c r="F93" s="38"/>
+      <c r="G93" s="38"/>
+      <c r="H93" s="38"/>
+      <c r="I93" s="38"/>
+      <c r="J93" s="38"/>
+      <c r="K93" s="38"/>
+      <c r="L93" s="38"/>
     </row>
     <row r="94" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="35" t="n">
+      <c r="A94" s="34" t="n">
         <v>2.67</v>
       </c>
-      <c r="B94" s="36" t="s">
+      <c r="B94" s="35" t="s">
         <v>135</v>
       </c>
-      <c r="C94" s="58" t="n">
+      <c r="C94" s="56" t="n">
         <v>50814</v>
       </c>
-      <c r="D94" s="40" t="s">
+      <c r="D94" s="39" t="s">
         <v>145</v>
       </c>
-      <c r="E94" s="40" t="s">
+      <c r="E94" s="39" t="s">
         <v>146</v>
       </c>
-      <c r="F94" s="39"/>
-      <c r="G94" s="39"/>
-      <c r="H94" s="39"/>
-      <c r="I94" s="39"/>
-      <c r="J94" s="39"/>
-      <c r="K94" s="39"/>
-      <c r="L94" s="39"/>
+      <c r="F94" s="38"/>
+      <c r="G94" s="38"/>
+      <c r="H94" s="38"/>
+      <c r="I94" s="38"/>
+      <c r="J94" s="38"/>
+      <c r="K94" s="38"/>
+      <c r="L94" s="38"/>
     </row>
     <row r="95" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="35" t="n">
+      <c r="A95" s="34" t="n">
         <v>2.67</v>
       </c>
-      <c r="B95" s="36" t="s">
+      <c r="B95" s="35" t="s">
         <v>135</v>
       </c>
-      <c r="C95" s="37" t="n">
+      <c r="C95" s="36" t="n">
         <v>50815</v>
       </c>
-      <c r="D95" s="40" t="s">
+      <c r="D95" s="39" t="s">
         <v>147</v>
       </c>
-      <c r="E95" s="40" t="s">
+      <c r="E95" s="39" t="s">
         <v>148</v>
       </c>
-      <c r="F95" s="39"/>
-      <c r="G95" s="39"/>
-      <c r="H95" s="39"/>
-      <c r="I95" s="39"/>
-      <c r="J95" s="39"/>
-      <c r="K95" s="39"/>
-      <c r="L95" s="39"/>
+      <c r="F95" s="38"/>
+      <c r="G95" s="38"/>
+      <c r="H95" s="38"/>
+      <c r="I95" s="38"/>
+      <c r="J95" s="38"/>
+      <c r="K95" s="38"/>
+      <c r="L95" s="38"/>
     </row>
     <row r="96" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="35"/>
-      <c r="B96" s="36"/>
-      <c r="C96" s="59" t="s">
+      <c r="A96" s="34"/>
+      <c r="B96" s="35"/>
+      <c r="C96" s="57" t="s">
         <v>149</v>
       </c>
-      <c r="D96" s="59"/>
-      <c r="E96" s="59"/>
-      <c r="F96" s="59"/>
-      <c r="G96" s="59"/>
-      <c r="H96" s="59"/>
-      <c r="I96" s="59"/>
-      <c r="J96" s="59"/>
-      <c r="K96" s="59"/>
-      <c r="L96" s="59"/>
+      <c r="D96" s="57"/>
+      <c r="E96" s="57"/>
+      <c r="F96" s="57"/>
+      <c r="G96" s="57"/>
+      <c r="H96" s="57"/>
+      <c r="I96" s="57"/>
+      <c r="J96" s="57"/>
+      <c r="K96" s="57"/>
+      <c r="L96" s="57"/>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="35"/>
-      <c r="B97" s="36"/>
-      <c r="C97" s="48"/>
-      <c r="D97" s="49" t="s">
+      <c r="A97" s="34"/>
+      <c r="B97" s="35"/>
+      <c r="C97" s="47"/>
+      <c r="D97" s="48" t="s">
         <v>150</v>
       </c>
-      <c r="E97" s="50"/>
-      <c r="F97" s="41"/>
-      <c r="G97" s="42"/>
-      <c r="H97" s="42"/>
-      <c r="I97" s="42"/>
-      <c r="J97" s="41"/>
-      <c r="K97" s="42"/>
-      <c r="L97" s="41"/>
+      <c r="E97" s="49"/>
+      <c r="F97" s="40"/>
+      <c r="G97" s="41"/>
+      <c r="H97" s="41"/>
+      <c r="I97" s="41"/>
+      <c r="J97" s="40"/>
+      <c r="K97" s="41"/>
+      <c r="L97" s="40"/>
     </row>
     <row r="98" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="35" t="n">
+      <c r="A98" s="34" t="n">
         <v>2.43</v>
       </c>
-      <c r="B98" s="36" t="s">
+      <c r="B98" s="35" t="s">
         <v>151</v>
       </c>
-      <c r="C98" s="60" t="n">
+      <c r="C98" s="36" t="n">
         <v>50789</v>
       </c>
-      <c r="D98" s="61" t="s">
+      <c r="D98" s="39" t="s">
         <v>152</v>
       </c>
-      <c r="E98" s="62" t="s">
+      <c r="E98" s="58" t="s">
         <v>153</v>
       </c>
-      <c r="F98" s="39"/>
-      <c r="G98" s="39"/>
-      <c r="H98" s="39"/>
-      <c r="I98" s="39"/>
-      <c r="J98" s="39"/>
-      <c r="K98" s="39"/>
-      <c r="L98" s="39"/>
+      <c r="F98" s="38"/>
+      <c r="G98" s="38"/>
+      <c r="H98" s="38"/>
+      <c r="I98" s="38"/>
+      <c r="J98" s="38"/>
+      <c r="K98" s="38"/>
+      <c r="L98" s="38"/>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="35"/>
-      <c r="B99" s="36"/>
-      <c r="C99" s="48"/>
-      <c r="D99" s="49" t="s">
+      <c r="A99" s="34"/>
+      <c r="B99" s="35"/>
+      <c r="C99" s="47"/>
+      <c r="D99" s="48" t="s">
         <v>154</v>
       </c>
-      <c r="E99" s="50"/>
-      <c r="F99" s="41"/>
-      <c r="G99" s="42"/>
-      <c r="H99" s="42"/>
-      <c r="I99" s="42"/>
-      <c r="J99" s="41"/>
-      <c r="K99" s="42"/>
-      <c r="L99" s="41"/>
+      <c r="E99" s="49"/>
+      <c r="F99" s="40"/>
+      <c r="G99" s="41"/>
+      <c r="H99" s="41"/>
+      <c r="I99" s="41"/>
+      <c r="J99" s="40"/>
+      <c r="K99" s="41"/>
+      <c r="L99" s="40"/>
     </row>
     <row r="100" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="35" t="n">
+      <c r="A100" s="34" t="n">
         <v>2.75</v>
       </c>
-      <c r="B100" s="36" t="s">
+      <c r="B100" s="35" t="s">
         <v>151</v>
       </c>
-      <c r="C100" s="60" t="n">
+      <c r="C100" s="36" t="n">
         <v>50790</v>
       </c>
-      <c r="D100" s="61" t="s">
+      <c r="D100" s="39" t="s">
         <v>155</v>
       </c>
-      <c r="E100" s="63" t="s">
+      <c r="E100" s="59" t="s">
         <v>156</v>
       </c>
-      <c r="F100" s="64"/>
-      <c r="G100" s="64"/>
-      <c r="H100" s="64"/>
-      <c r="I100" s="64"/>
-      <c r="J100" s="64"/>
-      <c r="K100" s="64"/>
-      <c r="L100" s="64"/>
-    </row>
-    <row r="101" s="67" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="35" t="n">
+      <c r="F100" s="60"/>
+      <c r="G100" s="60"/>
+      <c r="H100" s="60"/>
+      <c r="I100" s="60"/>
+      <c r="J100" s="60"/>
+      <c r="K100" s="60"/>
+      <c r="L100" s="60"/>
+    </row>
+    <row r="101" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="34" t="n">
         <v>2.39</v>
       </c>
-      <c r="B101" s="65" t="s">
+      <c r="B101" s="35" t="s">
         <v>151</v>
       </c>
-      <c r="C101" s="37" t="n">
+      <c r="C101" s="36" t="n">
         <v>50799</v>
       </c>
-      <c r="D101" s="40" t="s">
+      <c r="D101" s="39" t="s">
         <v>157</v>
       </c>
-      <c r="E101" s="63" t="s">
+      <c r="E101" s="59" t="s">
         <v>158</v>
       </c>
-      <c r="F101" s="66"/>
-      <c r="G101" s="66"/>
-      <c r="H101" s="66"/>
-      <c r="I101" s="66"/>
-      <c r="J101" s="66"/>
-      <c r="K101" s="66"/>
-      <c r="L101" s="66"/>
+      <c r="F101" s="60"/>
+      <c r="G101" s="60"/>
+      <c r="H101" s="60"/>
+      <c r="I101" s="60"/>
+      <c r="J101" s="60"/>
+      <c r="K101" s="60"/>
+      <c r="L101" s="60"/>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="35"/>
-      <c r="B102" s="65"/>
-      <c r="C102" s="68"/>
-      <c r="D102" s="69" t="s">
+      <c r="A102" s="34"/>
+      <c r="B102" s="35"/>
+      <c r="C102" s="47"/>
+      <c r="D102" s="48" t="s">
         <v>159</v>
       </c>
-      <c r="E102" s="70"/>
-      <c r="F102" s="71"/>
-      <c r="G102" s="72"/>
-      <c r="H102" s="72"/>
-      <c r="I102" s="72"/>
-      <c r="J102" s="71"/>
-      <c r="K102" s="72"/>
-      <c r="L102" s="71"/>
+      <c r="E102" s="49"/>
+      <c r="F102" s="40"/>
+      <c r="G102" s="41"/>
+      <c r="H102" s="41"/>
+      <c r="I102" s="41"/>
+      <c r="J102" s="40"/>
+      <c r="K102" s="41"/>
+      <c r="L102" s="40"/>
     </row>
     <row r="103" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="35" t="n">
+      <c r="A103" s="34" t="n">
         <v>3.1</v>
       </c>
-      <c r="B103" s="65" t="s">
+      <c r="B103" s="35" t="s">
         <v>151</v>
       </c>
-      <c r="C103" s="37" t="n">
+      <c r="C103" s="36" t="n">
         <v>50792</v>
       </c>
-      <c r="D103" s="40" t="s">
+      <c r="D103" s="39" t="s">
         <v>160</v>
       </c>
-      <c r="E103" s="63" t="s">
+      <c r="E103" s="59" t="s">
         <v>161</v>
       </c>
-      <c r="F103" s="66"/>
-      <c r="G103" s="66"/>
-      <c r="H103" s="66"/>
-      <c r="I103" s="66"/>
-      <c r="J103" s="66"/>
-      <c r="K103" s="66"/>
-      <c r="L103" s="66"/>
+      <c r="F103" s="60"/>
+      <c r="G103" s="60"/>
+      <c r="H103" s="60"/>
+      <c r="I103" s="60"/>
+      <c r="J103" s="60"/>
+      <c r="K103" s="60"/>
+      <c r="L103" s="60"/>
     </row>
     <row r="104" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="35" t="n">
+      <c r="A104" s="34" t="n">
         <v>2.85</v>
       </c>
-      <c r="B104" s="65" t="s">
+      <c r="B104" s="35" t="s">
         <v>151</v>
       </c>
-      <c r="C104" s="37" t="n">
+      <c r="C104" s="36" t="n">
         <v>50798</v>
       </c>
-      <c r="D104" s="40" t="s">
+      <c r="D104" s="39" t="s">
         <v>162</v>
       </c>
-      <c r="E104" s="63" t="s">
+      <c r="E104" s="59" t="s">
         <v>163</v>
       </c>
-      <c r="F104" s="66"/>
-      <c r="G104" s="66"/>
-      <c r="H104" s="66"/>
-      <c r="I104" s="66"/>
-      <c r="J104" s="66"/>
-      <c r="K104" s="66"/>
-      <c r="L104" s="66"/>
+      <c r="F104" s="60"/>
+      <c r="G104" s="60"/>
+      <c r="H104" s="60"/>
+      <c r="I104" s="60"/>
+      <c r="J104" s="60"/>
+      <c r="K104" s="60"/>
+      <c r="L104" s="60"/>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="35"/>
-      <c r="B105" s="65"/>
-      <c r="C105" s="68"/>
-      <c r="D105" s="69" t="s">
+      <c r="A105" s="34"/>
+      <c r="B105" s="35"/>
+      <c r="C105" s="47"/>
+      <c r="D105" s="48" t="s">
         <v>96</v>
       </c>
-      <c r="E105" s="70"/>
-      <c r="F105" s="71"/>
-      <c r="G105" s="72"/>
-      <c r="H105" s="72"/>
-      <c r="I105" s="72"/>
-      <c r="J105" s="71"/>
-      <c r="K105" s="72"/>
-      <c r="L105" s="71"/>
+      <c r="E105" s="49"/>
+      <c r="F105" s="40"/>
+      <c r="G105" s="41"/>
+      <c r="H105" s="41"/>
+      <c r="I105" s="41"/>
+      <c r="J105" s="40"/>
+      <c r="K105" s="41"/>
+      <c r="L105" s="40"/>
     </row>
     <row r="106" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="35" t="n">
+      <c r="A106" s="34" t="n">
         <v>2.65</v>
       </c>
-      <c r="B106" s="65" t="s">
+      <c r="B106" s="35" t="s">
         <v>151</v>
       </c>
-      <c r="C106" s="37" t="n">
+      <c r="C106" s="36" t="n">
         <v>50791</v>
       </c>
-      <c r="D106" s="40" t="s">
+      <c r="D106" s="39" t="s">
         <v>164</v>
       </c>
-      <c r="E106" s="63" t="s">
+      <c r="E106" s="59" t="s">
         <v>165</v>
       </c>
-      <c r="F106" s="66"/>
-      <c r="G106" s="66"/>
-      <c r="H106" s="66"/>
-      <c r="I106" s="66"/>
-      <c r="J106" s="66"/>
-      <c r="K106" s="66"/>
-      <c r="L106" s="66"/>
+      <c r="F106" s="60"/>
+      <c r="G106" s="60"/>
+      <c r="H106" s="60"/>
+      <c r="I106" s="60"/>
+      <c r="J106" s="60"/>
+      <c r="K106" s="60"/>
+      <c r="L106" s="60"/>
     </row>
     <row r="107" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="35" t="n">
+      <c r="A107" s="34" t="n">
         <v>2.88</v>
       </c>
-      <c r="B107" s="65" t="s">
+      <c r="B107" s="35" t="s">
         <v>151</v>
       </c>
-      <c r="C107" s="37" t="n">
+      <c r="C107" s="36" t="n">
         <v>50800</v>
       </c>
-      <c r="D107" s="73" t="s">
+      <c r="D107" s="61" t="s">
         <v>166</v>
       </c>
-      <c r="E107" s="63" t="s">
+      <c r="E107" s="59" t="s">
         <v>73</v>
       </c>
-      <c r="F107" s="66"/>
-      <c r="G107" s="66"/>
-      <c r="H107" s="66"/>
-      <c r="I107" s="66"/>
-      <c r="J107" s="66"/>
-      <c r="K107" s="66"/>
-      <c r="L107" s="66"/>
+      <c r="F107" s="60"/>
+      <c r="G107" s="60"/>
+      <c r="H107" s="60"/>
+      <c r="I107" s="60"/>
+      <c r="J107" s="60"/>
+      <c r="K107" s="60"/>
+      <c r="L107" s="60"/>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="35"/>
-      <c r="B108" s="65"/>
-      <c r="C108" s="68"/>
-      <c r="D108" s="69" t="s">
+      <c r="A108" s="34"/>
+      <c r="B108" s="35"/>
+      <c r="C108" s="47"/>
+      <c r="D108" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="E108" s="70"/>
-      <c r="F108" s="71"/>
-      <c r="G108" s="72"/>
-      <c r="H108" s="72"/>
-      <c r="I108" s="72"/>
-      <c r="J108" s="71"/>
-      <c r="K108" s="72"/>
-      <c r="L108" s="71"/>
+      <c r="E108" s="49"/>
+      <c r="F108" s="40"/>
+      <c r="G108" s="41"/>
+      <c r="H108" s="41"/>
+      <c r="I108" s="41"/>
+      <c r="J108" s="40"/>
+      <c r="K108" s="41"/>
+      <c r="L108" s="40"/>
     </row>
     <row r="109" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="35" t="n">
+      <c r="A109" s="34" t="n">
         <v>2.3</v>
       </c>
-      <c r="B109" s="65" t="s">
+      <c r="B109" s="35" t="s">
         <v>151</v>
       </c>
-      <c r="C109" s="37" t="n">
+      <c r="C109" s="36" t="n">
         <v>50793</v>
       </c>
-      <c r="D109" s="40" t="s">
+      <c r="D109" s="39" t="s">
         <v>167</v>
       </c>
-      <c r="E109" s="63" t="s">
+      <c r="E109" s="59" t="s">
         <v>168</v>
       </c>
-      <c r="F109" s="66"/>
-      <c r="G109" s="66"/>
-      <c r="H109" s="66"/>
-      <c r="I109" s="66"/>
-      <c r="J109" s="66"/>
-      <c r="K109" s="66"/>
-      <c r="L109" s="66"/>
+      <c r="F109" s="60"/>
+      <c r="G109" s="60"/>
+      <c r="H109" s="60"/>
+      <c r="I109" s="60"/>
+      <c r="J109" s="60"/>
+      <c r="K109" s="60"/>
+      <c r="L109" s="60"/>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="35"/>
-      <c r="B110" s="36"/>
-      <c r="C110" s="48"/>
-      <c r="D110" s="49" t="s">
+      <c r="A110" s="34"/>
+      <c r="B110" s="35"/>
+      <c r="C110" s="47"/>
+      <c r="D110" s="48" t="s">
         <v>169</v>
       </c>
-      <c r="E110" s="50"/>
-      <c r="F110" s="41"/>
-      <c r="G110" s="42"/>
-      <c r="H110" s="42"/>
-      <c r="I110" s="42"/>
-      <c r="J110" s="41"/>
-      <c r="K110" s="42"/>
-      <c r="L110" s="41"/>
+      <c r="E110" s="49"/>
+      <c r="F110" s="40"/>
+      <c r="G110" s="41"/>
+      <c r="H110" s="41"/>
+      <c r="I110" s="41"/>
+      <c r="J110" s="40"/>
+      <c r="K110" s="41"/>
+      <c r="L110" s="40"/>
     </row>
     <row r="111" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="35" t="n">
+      <c r="A111" s="34" t="n">
         <v>2.5</v>
       </c>
-      <c r="B111" s="36" t="s">
+      <c r="B111" s="35" t="s">
         <v>151</v>
       </c>
-      <c r="C111" s="60" t="n">
+      <c r="C111" s="36" t="n">
         <v>50794</v>
       </c>
-      <c r="D111" s="61" t="s">
+      <c r="D111" s="39" t="s">
         <v>170</v>
       </c>
-      <c r="E111" s="63" t="s">
+      <c r="E111" s="59" t="s">
         <v>171</v>
       </c>
-      <c r="F111" s="39"/>
-      <c r="G111" s="39"/>
-      <c r="H111" s="39"/>
-      <c r="I111" s="39"/>
-      <c r="J111" s="39"/>
-      <c r="K111" s="39"/>
-      <c r="L111" s="39"/>
+      <c r="F111" s="38"/>
+      <c r="G111" s="38"/>
+      <c r="H111" s="38"/>
+      <c r="I111" s="38"/>
+      <c r="J111" s="38"/>
+      <c r="K111" s="38"/>
+      <c r="L111" s="38"/>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="35"/>
-      <c r="B112" s="36"/>
-      <c r="C112" s="48"/>
-      <c r="D112" s="49" t="s">
+      <c r="A112" s="34"/>
+      <c r="B112" s="35"/>
+      <c r="C112" s="47"/>
+      <c r="D112" s="48" t="s">
         <v>172</v>
       </c>
-      <c r="E112" s="50"/>
-      <c r="F112" s="41"/>
-      <c r="G112" s="42"/>
-      <c r="H112" s="42"/>
-      <c r="I112" s="42"/>
-      <c r="J112" s="41"/>
-      <c r="K112" s="42"/>
-      <c r="L112" s="41"/>
+      <c r="E112" s="49"/>
+      <c r="F112" s="40"/>
+      <c r="G112" s="41"/>
+      <c r="H112" s="41"/>
+      <c r="I112" s="41"/>
+      <c r="J112" s="40"/>
+      <c r="K112" s="41"/>
+      <c r="L112" s="40"/>
     </row>
     <row r="113" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="35" t="n">
+      <c r="A113" s="34" t="n">
         <v>2.76</v>
       </c>
-      <c r="B113" s="36" t="s">
+      <c r="B113" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C113" s="74" t="n">
+      <c r="C113" s="62" t="n">
         <v>50806</v>
       </c>
-      <c r="D113" s="61" t="s">
+      <c r="D113" s="39" t="s">
         <v>173</v>
       </c>
-      <c r="E113" s="63" t="s">
+      <c r="E113" s="59" t="s">
         <v>174</v>
       </c>
-      <c r="F113" s="39"/>
-      <c r="G113" s="39"/>
-      <c r="H113" s="39"/>
-      <c r="I113" s="39"/>
-      <c r="J113" s="39"/>
-      <c r="K113" s="39"/>
-      <c r="L113" s="39"/>
+      <c r="F113" s="38"/>
+      <c r="G113" s="38"/>
+      <c r="H113" s="38"/>
+      <c r="I113" s="38"/>
+      <c r="J113" s="38"/>
+      <c r="K113" s="38"/>
+      <c r="L113" s="38"/>
     </row>
     <row r="114" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="35" t="n">
+      <c r="A114" s="34" t="n">
         <v>2.76</v>
       </c>
-      <c r="B114" s="36" t="s">
+      <c r="B114" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C114" s="37" t="n">
+      <c r="C114" s="36" t="n">
         <v>50816</v>
       </c>
-      <c r="D114" s="61" t="s">
+      <c r="D114" s="39" t="s">
         <v>175</v>
       </c>
-      <c r="E114" s="63" t="s">
+      <c r="E114" s="59" t="s">
         <v>174</v>
       </c>
-      <c r="F114" s="39"/>
-      <c r="G114" s="39"/>
-      <c r="H114" s="39"/>
-      <c r="I114" s="39"/>
-      <c r="J114" s="39"/>
-      <c r="K114" s="39"/>
-      <c r="L114" s="39"/>
+      <c r="F114" s="38"/>
+      <c r="G114" s="38"/>
+      <c r="H114" s="38"/>
+      <c r="I114" s="38"/>
+      <c r="J114" s="38"/>
+      <c r="K114" s="38"/>
+      <c r="L114" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>